<commit_message>
Fixed some little things in data formation loop re: having changed config file to excel instead of csv.
Started on producing graph averages. In the process, rearranged so conditional parts of graph formation code are in packages near each other - moved inputs into conditional parts next to code that actually adds them to graph.
</commit_message>
<xml_diff>
--- a/graph_configs.xlsx
+++ b/graph_configs.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,10 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WNF\Documents\GIT PROJECTS\CWIS-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{F430FE64-E20F-41A5-B619-44BD81D7ADEA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B97210-4171-4003-8602-0F83978516D0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19920" windowHeight="7710"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="7710" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="7710" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
   </bookViews>
   <sheets>
     <sheet name="slide.types" sheetId="1" r:id="rId1"/>
@@ -19,6 +18,7 @@
     <sheet name="slide.objects" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">graph.types!$A$1:$L$10</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">slide.types!$A$1:$E$13</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="80">
   <si>
     <t>slide.type.id</t>
   </si>
@@ -136,9 +136,6 @@
     <t>graph.average</t>
   </si>
   <si>
-    <t>graph.avg.group.by.var</t>
-  </si>
-  <si>
     <t>graph.cat.varname</t>
   </si>
   <si>
@@ -191,9 +188,6 @@
   </si>
   <si>
     <t>year,module</t>
-  </si>
-  <si>
-    <t>year, module</t>
   </si>
   <si>
     <t>d</t>
@@ -277,7 +271,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1111,13 +1105,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1311,7 +1302,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E13">
+  <autoFilter ref="A1:E13" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState ref="A2:E13">
       <sortCondition ref="C1:C13"/>
     </sortState>
@@ -1321,17 +1312,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -1368,186 +1358,174 @@
       <c r="L1" t="s">
         <v>38</v>
       </c>
-      <c r="M1" t="s">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>40</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
       </c>
       <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
         <v>41</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>42</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>43</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>44</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>45</v>
       </c>
-      <c r="K2" t="s">
-        <v>46</v>
+      <c r="K2">
+        <v>0</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
         <v>47</v>
       </c>
-      <c r="B3" t="s">
-        <v>48</v>
-      </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J3" t="s">
         <v>49</v>
       </c>
-      <c r="K3" t="s">
-        <v>50</v>
+      <c r="K3">
+        <v>0</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
-      <c r="M3">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="L4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>54</v>
       </c>
-      <c r="I4" t="s">
-        <v>45</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="B5" t="s">
         <v>55</v>
       </c>
-      <c r="K4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" t="s">
-        <v>57</v>
-      </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J5" t="s">
-        <v>55</v>
-      </c>
-      <c r="K5" t="s">
         <v>22</v>
       </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
       <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I6" t="s">
         <v>58</v>
       </c>
-      <c r="C6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I6" t="s">
-        <v>60</v>
-      </c>
-      <c r="K6" t="s">
-        <v>59</v>
+      <c r="J6" t="s">
+        <v>57</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
       </c>
       <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="M6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1555,31 +1533,31 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
         <v>41</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>42</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>43</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>44</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>45</v>
       </c>
-      <c r="K7" t="s">
-        <v>46</v>
+      <c r="K7">
+        <v>1</v>
       </c>
       <c r="L7">
-        <v>1</v>
-      </c>
-      <c r="M7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1587,31 +1565,31 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G8" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" t="s">
         <v>44</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>45</v>
       </c>
-      <c r="K8" t="s">
-        <v>46</v>
+      <c r="K8">
+        <v>0</v>
       </c>
       <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1619,81 +1597,79 @@
         <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F9" t="s">
         <v>22</v>
       </c>
       <c r="G9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" t="s">
         <v>44</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>45</v>
       </c>
-      <c r="K9" t="s">
-        <v>46</v>
+      <c r="K9">
+        <v>0</v>
       </c>
       <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F10" t="s">
         <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I10" t="s">
-        <v>60</v>
-      </c>
-      <c r="K10" t="s">
-        <v>65</v>
+        <v>58</v>
+      </c>
+      <c r="J10" t="s">
+        <v>63</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
       </c>
       <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L10" xr:uid="{F761CE15-AF34-4E73-B732-AD7C7249D5C1}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1709,54 +1685,54 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" t="s">
         <v>67</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>68</v>
       </c>
-      <c r="D1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>69</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>70</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>71</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>72</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>73</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>74</v>
-      </c>
-      <c r="K1" t="s">
-        <v>75</v>
-      </c>
-      <c r="L1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F2">
         <v>0.2</v>
@@ -1771,13 +1747,13 @@
         <v>0.71</v>
       </c>
       <c r="J2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K2">
         <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked out averages. Now seems like messed up the measure.var, though, for some graphs. Also appears that for final graphs, the ones with agreement scales have a reverse order 1-5. Probably easiest to just recode in original data.
Started a little more work on making powerpoints.
</commit_message>
<xml_diff>
--- a/graph_configs.xlsx
+++ b/graph_configs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WNF\Documents\GIT PROJECTS\CWIS-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B97210-4171-4003-8602-0F83978516D0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54D3888-DA25-41AA-B665-E2319E42BC53}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="7710" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="7710" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
   </bookViews>
   <sheets>
     <sheet name="slide.types" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,21 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">graph.types!$A$1:$L$10</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">slide.types!$A$1:$E$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">slide.types!$A$1:$F$13</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="84">
   <si>
     <t>slide.type.id</t>
   </si>
@@ -223,9 +230,6 @@
     <t>placement.order</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -266,6 +270,21 @@
   </si>
   <si>
     <t>2,6,7,8,9,10,11,12</t>
+  </si>
+  <si>
+    <t>slide.layout</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>slide</t>
+  </si>
+  <si>
+    <t>section</t>
+  </si>
+  <si>
+    <t>object.id</t>
   </si>
 </sst>
 </file>
@@ -1106,20 +1125,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="2" width="40.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="3" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1130,13 +1151,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1146,8 +1170,11 @@
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1157,8 +1184,11 @@
       <c r="C3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6</v>
       </c>
@@ -1168,11 +1198,14 @@
       <c r="C4">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>7</v>
       </c>
@@ -1183,13 +1216,16 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1199,8 +1235,11 @@
       <c r="C6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>8</v>
       </c>
@@ -1210,11 +1249,14 @@
       <c r="C7">
         <v>6</v>
       </c>
-      <c r="E7" t="s">
+      <c r="D7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9</v>
       </c>
@@ -1224,11 +1266,14 @@
       <c r="C8">
         <v>7</v>
       </c>
-      <c r="E8" t="s">
+      <c r="D8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1238,8 +1283,11 @@
       <c r="C9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -1249,11 +1297,14 @@
       <c r="C10">
         <v>9</v>
       </c>
-      <c r="E10" t="s">
+      <c r="D10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
@@ -1264,13 +1315,16 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" t="s">
         <v>22</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
@@ -1281,10 +1335,13 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1295,15 +1352,18 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" t="s">
         <v>25</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E13" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState ref="A2:E13">
+  <autoFilter ref="A1:F13" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState ref="A2:F13">
       <sortCondition ref="C1:C13"/>
     </sortState>
   </autoFilter>
@@ -1315,7 +1375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -1669,13 +1729,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
   </cols>
@@ -1685,54 +1746,54 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" t="s">
         <v>65</v>
-      </c>
-      <c r="C1" t="s">
-        <v>66</v>
       </c>
       <c r="D1" t="s">
         <v>64</v>
       </c>
       <c r="E1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" t="s">
         <v>67</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>68</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>69</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>70</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>71</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>72</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>73</v>
-      </c>
-      <c r="L1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F2">
         <v>0.2</v>
@@ -1747,13 +1808,13 @@
         <v>0.71</v>
       </c>
       <c r="J2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K2">
         <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on adding piece-of-text objects in a loop. Then graphs, then finally the table.
</commit_message>
<xml_diff>
--- a/graph_configs.xlsx
+++ b/graph_configs.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WNF\Documents\GIT PROJECTS\CWIS-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54D3888-DA25-41AA-B665-E2319E42BC53}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C09D80-DFA7-4ABA-8D55-398DEA87345F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="7710" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
   </bookViews>
   <sheets>
     <sheet name="slide.types" sheetId="1" r:id="rId1"/>
     <sheet name="graph.types" sheetId="2" r:id="rId2"/>
-    <sheet name="slide.objects" sheetId="3" r:id="rId3"/>
+    <sheet name="slide.pot.objects" sheetId="3" r:id="rId3"/>
+    <sheet name="slide.table.objects" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">graph.types!$A$1:$L$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">slide.pot.objects!$A$1:$O$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">slide.types!$A$1:$F$13</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="101">
   <si>
     <t>slide.type.id</t>
   </si>
@@ -269,9 +271,6 @@
     <t>61,34,66</t>
   </si>
   <si>
-    <t>2,6,7,8,9,10,11,12</t>
-  </si>
-  <si>
     <t>slide.layout</t>
   </si>
   <si>
@@ -285,6 +284,60 @@
   </si>
   <si>
     <t>object.id</t>
+  </si>
+  <si>
+    <t>Presentation Notes</t>
+  </si>
+  <si>
+    <t>presentation.title.static</t>
+  </si>
+  <si>
+    <t>presentation.title.date</t>
+  </si>
+  <si>
+    <t>presentation.title</t>
+  </si>
+  <si>
+    <t>content.static</t>
+  </si>
+  <si>
+    <t>content.dynamic</t>
+  </si>
+  <si>
+    <t>presentation.subtitle</t>
+  </si>
+  <si>
+    <t>Repeated Measures Report</t>
+  </si>
+  <si>
+    <t>Baseline through 2017-18 SY</t>
+  </si>
+  <si>
+    <t>current.date</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>offx</t>
+  </si>
+  <si>
+    <t>offy</t>
+  </si>
+  <si>
+    <t>font.weight</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>text.align</t>
   </si>
 </sst>
 </file>
@@ -427,7 +480,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -605,6 +658,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -768,8 +827,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1128,7 +1189,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1151,7 +1212,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -1171,7 +1232,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1185,7 +1246,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1199,7 +1260,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
@@ -1216,7 +1277,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -1236,7 +1297,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1250,7 +1311,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F7" t="s">
         <v>16</v>
@@ -1267,7 +1328,7 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F8" t="s">
         <v>18</v>
@@ -1284,7 +1345,7 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1298,7 +1359,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F10" t="s">
         <v>20</v>
@@ -1315,7 +1376,7 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E11" t="s">
         <v>22</v>
@@ -1335,7 +1396,7 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1352,7 +1413,7 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E13" t="s">
         <v>25</v>
@@ -1727,10 +1788,293 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:O6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="4" max="16" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>7.76</v>
+      </c>
+      <c r="F2">
+        <v>0.85</v>
+      </c>
+      <c r="G2">
+        <v>1.27</v>
+      </c>
+      <c r="H2">
+        <v>2.78</v>
+      </c>
+      <c r="I2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J2">
+        <v>48</v>
+      </c>
+      <c r="L2" t="s">
+        <v>77</v>
+      </c>
+      <c r="M2" t="s">
+        <v>93</v>
+      </c>
+      <c r="N2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>4.67</v>
+      </c>
+      <c r="F3">
+        <v>0.61</v>
+      </c>
+      <c r="G3">
+        <v>1.27</v>
+      </c>
+      <c r="H3">
+        <v>3.66</v>
+      </c>
+      <c r="I3" t="s">
+        <v>76</v>
+      </c>
+      <c r="J3">
+        <v>30</v>
+      </c>
+      <c r="L3" t="s">
+        <v>77</v>
+      </c>
+      <c r="M3" t="s">
+        <v>93</v>
+      </c>
+      <c r="N3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>7.76</v>
+      </c>
+      <c r="F4">
+        <v>0.67</v>
+      </c>
+      <c r="G4">
+        <v>1.27</v>
+      </c>
+      <c r="H4">
+        <v>5.4</v>
+      </c>
+      <c r="I4" t="s">
+        <v>76</v>
+      </c>
+      <c r="J4">
+        <v>28</v>
+      </c>
+      <c r="L4" s="2" t="str">
+        <f>"202,202,202"</f>
+        <v>202,202,202</v>
+      </c>
+      <c r="M4" t="s">
+        <v>93</v>
+      </c>
+      <c r="O4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>7.76</v>
+      </c>
+      <c r="F5">
+        <v>0.67</v>
+      </c>
+      <c r="G5">
+        <v>1.27</v>
+      </c>
+      <c r="H5">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="I5" t="s">
+        <v>76</v>
+      </c>
+      <c r="J5">
+        <v>28</v>
+      </c>
+      <c r="L5" t="s">
+        <v>77</v>
+      </c>
+      <c r="M5" t="s">
+        <v>93</v>
+      </c>
+      <c r="N5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>9.2100000000000009</v>
+      </c>
+      <c r="F6">
+        <v>0.71</v>
+      </c>
+      <c r="G6">
+        <v>0.2</v>
+      </c>
+      <c r="H6">
+        <v>0.2</v>
+      </c>
+      <c r="I6" t="s">
+        <v>76</v>
+      </c>
+      <c r="J6">
+        <v>30</v>
+      </c>
+      <c r="L6" t="s">
+        <v>77</v>
+      </c>
+      <c r="M6" t="s">
+        <v>93</v>
+      </c>
+      <c r="N6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:O6" xr:uid="{AAFC98FD-2B31-46F6-BF19-8C5861C2C493}">
+    <sortState ref="A2:O6">
+      <sortCondition ref="B1:B5"/>
+    </sortState>
+  </autoFilter>
+  <sortState ref="A2:O6">
+    <sortCondition ref="A2:A6"/>
+    <sortCondition ref="D2:D6"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8346032C-9F0F-4902-A148-43BA06579F87}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1746,7 +2090,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C1" t="s">
         <v>65</v>
@@ -1780,8 +2124,8 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>78</v>
+      <c r="A2">
+        <v>2</v>
       </c>
       <c r="B2">
         <v>1</v>

</xml_diff>

<commit_message>
Have been working on making full list of slides with little success. Have designed database-ish diagram in lucidcharts and now going to work within data production loop ('b') to modify 'c' loop to produce full list of slides.
</commit_message>
<xml_diff>
--- a/graph_configs.xlsx
+++ b/graph_configs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WNF\Documents\GIT PROJECTS\CWIS-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C09D80-DFA7-4ABA-8D55-398DEA87345F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A31A2C-F8B2-49F4-9CA8-5A263B1D673D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="7710" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="116">
   <si>
     <t>slide.type.id</t>
   </si>
@@ -313,9 +313,6 @@
     <t>Baseline through 2017-18 SY</t>
   </si>
   <si>
-    <t>current.date</t>
-  </si>
-  <si>
     <t>left</t>
   </si>
   <si>
@@ -338,6 +335,54 @@
   </si>
   <si>
     <t>text.align</t>
+  </si>
+  <si>
+    <t>format(Sys.Date(), format = "%d-%b-%Y")</t>
+  </si>
+  <si>
+    <t>presentation.notes</t>
+  </si>
+  <si>
+    <t>bold</t>
+  </si>
+  <si>
+    <t>district.ids[h]</t>
+  </si>
+  <si>
+    <t>blah, blah, blah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">District: </t>
+  </si>
+  <si>
+    <t>Participation (CWIS Responses)</t>
+  </si>
+  <si>
+    <t>Performance: Implementation Rates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">District Dashboard: </t>
+  </si>
+  <si>
+    <t>graph.title.1</t>
+  </si>
+  <si>
+    <t>graph.title.2</t>
+  </si>
+  <si>
+    <t>footer</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>49,49,38</t>
+  </si>
+  <si>
+    <t>School Dashboard:</t>
+  </si>
+  <si>
+    <t>slides.df.h$school[i]</t>
   </si>
 </sst>
 </file>
@@ -1189,7 +1234,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1788,18 +1833,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
+      <selection pane="bottomLeft" activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="16" width="11.28515625" customWidth="1"/>
+    <col min="4" max="13" width="11.28515625" customWidth="1"/>
+    <col min="14" max="14" width="35" customWidth="1"/>
+    <col min="15" max="15" width="38.5703125" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1819,13 +1867,13 @@
         <v>94</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>71</v>
@@ -1834,13 +1882,13 @@
         <v>72</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>87</v>
@@ -1863,10 +1911,10 @@
         <v>1</v>
       </c>
       <c r="E2">
+        <v>0.85</v>
+      </c>
+      <c r="F2">
         <v>7.76</v>
-      </c>
-      <c r="F2">
-        <v>0.85</v>
       </c>
       <c r="G2">
         <v>1.27</v>
@@ -1880,11 +1928,14 @@
       <c r="J2">
         <v>48</v>
       </c>
+      <c r="K2" t="s">
+        <v>102</v>
+      </c>
       <c r="L2" t="s">
         <v>77</v>
       </c>
       <c r="M2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N2" t="s">
         <v>90</v>
@@ -1904,10 +1955,10 @@
         <v>4</v>
       </c>
       <c r="E3">
-        <v>4.67</v>
+        <v>0.61</v>
       </c>
       <c r="F3">
-        <v>0.61</v>
+        <v>7.76</v>
       </c>
       <c r="G3">
         <v>1.27</v>
@@ -1925,7 +1976,7 @@
         <v>77</v>
       </c>
       <c r="M3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N3" t="s">
         <v>91</v>
@@ -1945,10 +1996,10 @@
         <v>2</v>
       </c>
       <c r="E4">
+        <v>0.67</v>
+      </c>
+      <c r="F4">
         <v>7.76</v>
-      </c>
-      <c r="F4">
-        <v>0.67</v>
       </c>
       <c r="G4">
         <v>1.27</v>
@@ -1967,10 +2018,10 @@
         <v>202,202,202</v>
       </c>
       <c r="M4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O4" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1987,10 +2038,10 @@
         <v>3</v>
       </c>
       <c r="E5">
+        <v>0.67</v>
+      </c>
+      <c r="F5">
         <v>7.76</v>
-      </c>
-      <c r="F5">
-        <v>0.67</v>
       </c>
       <c r="G5">
         <v>1.27</v>
@@ -2004,14 +2055,20 @@
       <c r="J5">
         <v>28</v>
       </c>
+      <c r="K5" t="s">
+        <v>102</v>
+      </c>
       <c r="L5" t="s">
         <v>77</v>
       </c>
       <c r="M5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N5" t="s">
-        <v>90</v>
+        <v>105</v>
+      </c>
+      <c r="O5" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -2028,10 +2085,10 @@
         <v>1</v>
       </c>
       <c r="E6">
+        <v>0.71</v>
+      </c>
+      <c r="F6">
         <v>9.2100000000000009</v>
-      </c>
-      <c r="F6">
-        <v>0.71</v>
       </c>
       <c r="G6">
         <v>0.2</v>
@@ -2049,10 +2106,275 @@
         <v>77</v>
       </c>
       <c r="M6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N6" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F7">
+        <v>8.5500000000000007</v>
+      </c>
+      <c r="G7">
+        <v>0.62</v>
+      </c>
+      <c r="H7">
+        <v>1.55</v>
+      </c>
+      <c r="I7" t="s">
+        <v>76</v>
+      </c>
+      <c r="J7">
+        <v>20</v>
+      </c>
+      <c r="M7" t="s">
+        <v>92</v>
+      </c>
+      <c r="N7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0.71</v>
+      </c>
+      <c r="F8">
+        <v>9.2100000000000009</v>
+      </c>
+      <c r="G8">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H8">
+        <v>0.2</v>
+      </c>
+      <c r="I8" t="s">
+        <v>76</v>
+      </c>
+      <c r="J8">
+        <v>30</v>
+      </c>
+      <c r="K8" t="s">
+        <v>102</v>
+      </c>
+      <c r="L8" t="s">
+        <v>77</v>
+      </c>
+      <c r="M8" t="s">
+        <v>92</v>
+      </c>
+      <c r="N8" t="s">
+        <v>108</v>
+      </c>
+      <c r="O8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>0.67</v>
+      </c>
+      <c r="F9">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G9">
+        <v>0.36</v>
+      </c>
+      <c r="H9">
+        <v>0.79</v>
+      </c>
+      <c r="I9" t="s">
+        <v>76</v>
+      </c>
+      <c r="J9">
+        <v>18</v>
+      </c>
+      <c r="K9" t="s">
+        <v>102</v>
+      </c>
+      <c r="L9" t="s">
+        <v>113</v>
+      </c>
+      <c r="M9" t="s">
+        <v>92</v>
+      </c>
+      <c r="N9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>0.67</v>
+      </c>
+      <c r="F10">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G10">
+        <v>5.08</v>
+      </c>
+      <c r="H10">
+        <v>0.79</v>
+      </c>
+      <c r="I10" t="s">
+        <v>76</v>
+      </c>
+      <c r="J10">
+        <v>18</v>
+      </c>
+      <c r="K10" t="s">
+        <v>102</v>
+      </c>
+      <c r="L10" t="s">
+        <v>113</v>
+      </c>
+      <c r="M10" t="s">
+        <v>92</v>
+      </c>
+      <c r="N10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>0.34</v>
+      </c>
+      <c r="F11">
+        <v>2.31</v>
+      </c>
+      <c r="G11">
+        <v>6.73</v>
+      </c>
+      <c r="H11">
+        <v>6.78</v>
+      </c>
+      <c r="I11" t="s">
+        <v>76</v>
+      </c>
+      <c r="J11">
+        <v>14</v>
+      </c>
+      <c r="K11" t="s">
+        <v>102</v>
+      </c>
+      <c r="L11" s="2" t="str">
+        <f>"202,202,202"</f>
+        <v>202,202,202</v>
+      </c>
+      <c r="M11" t="s">
+        <v>112</v>
+      </c>
+      <c r="O11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0.71</v>
+      </c>
+      <c r="F12">
+        <v>9.2100000000000009</v>
+      </c>
+      <c r="G12">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H12">
+        <v>0.2</v>
+      </c>
+      <c r="I12" t="s">
+        <v>76</v>
+      </c>
+      <c r="J12">
+        <v>30</v>
+      </c>
+      <c r="K12" t="s">
+        <v>102</v>
+      </c>
+      <c r="L12" t="s">
+        <v>77</v>
+      </c>
+      <c r="M12" t="s">
+        <v>92</v>
+      </c>
+      <c r="N12" t="s">
+        <v>114</v>
+      </c>
+      <c r="O12" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2066,6 +2388,7 @@
     <sortCondition ref="D2:D6"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Loop expansion function appears to be working for at least one 'b' loop.
</commit_message>
<xml_diff>
--- a/graph_configs.xlsx
+++ b/graph_configs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WNF\Documents\GIT PROJECTS\CWIS-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A31A2C-F8B2-49F4-9CA8-5A263B1D673D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8796452-B1F6-48E0-BACA-7126FE0B4C35}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="7710" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="7710" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
   </bookViews>
   <sheets>
     <sheet name="slide.types" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="slide.table.objects" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">graph.types!$A$1:$L$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">graph.types!$A$1:$K$10</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">slide.pot.objects!$A$1:$O$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">slide.types!$A$1:$F$13</definedName>
   </definedNames>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="115">
   <si>
     <t>slide.type.id</t>
   </si>
@@ -137,9 +137,6 @@
   </si>
   <si>
     <t>data.group.by.var</t>
-  </si>
-  <si>
-    <t>graph.group.by.order</t>
   </si>
   <si>
     <t>graph.average</t>
@@ -1234,7 +1231,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1257,7 +1254,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -1277,7 +1274,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1291,7 +1288,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1305,7 +1302,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
@@ -1322,7 +1319,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -1342,7 +1339,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1356,7 +1353,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F7" t="s">
         <v>16</v>
@@ -1373,7 +1370,7 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F8" t="s">
         <v>18</v>
@@ -1390,7 +1387,7 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1404,7 +1401,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F10" t="s">
         <v>20</v>
@@ -1421,7 +1418,7 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E11" t="s">
         <v>22</v>
@@ -1441,7 +1438,7 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1458,7 +1455,7 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E13" t="s">
         <v>25</v>
@@ -1479,15 +1476,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -1521,177 +1518,174 @@
       <c r="K1" t="s">
         <v>37</v>
       </c>
-      <c r="L1" t="s">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>39</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
       </c>
       <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
         <v>40</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>41</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>42</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>43</v>
       </c>
       <c r="I2" t="s">
         <v>44</v>
       </c>
-      <c r="J2" t="s">
-        <v>45</v>
+      <c r="J2">
+        <v>0</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
         <v>46</v>
       </c>
-      <c r="B3" t="s">
-        <v>47</v>
-      </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
       </c>
       <c r="G3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" t="s">
         <v>48</v>
       </c>
-      <c r="I3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J3" t="s">
-        <v>49</v>
+      <c r="J3">
+        <v>0</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
-      <c r="L3">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="K4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>53</v>
       </c>
-      <c r="I4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>54</v>
       </c>
-      <c r="B5" t="s">
-        <v>55</v>
-      </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="H5" t="s">
+        <v>43</v>
       </c>
       <c r="I5" t="s">
-        <v>44</v>
-      </c>
-      <c r="J5" t="s">
         <v>22</v>
       </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
       <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" t="s">
         <v>56</v>
       </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>57</v>
       </c>
       <c r="I6" t="s">
-        <v>58</v>
-      </c>
-      <c r="J6" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
       </c>
       <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1699,31 +1693,31 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
         <v>40</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>41</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>42</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>43</v>
       </c>
       <c r="I7" t="s">
         <v>44</v>
       </c>
-      <c r="J7" t="s">
-        <v>45</v>
+      <c r="J7">
+        <v>1</v>
       </c>
       <c r="K7">
-        <v>1</v>
-      </c>
-      <c r="L7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1731,31 +1725,31 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" t="s">
         <v>43</v>
       </c>
       <c r="I8" t="s">
         <v>44</v>
       </c>
-      <c r="J8" t="s">
-        <v>45</v>
+      <c r="J8">
+        <v>0</v>
       </c>
       <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1763,70 +1757,70 @@
         <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F9" t="s">
         <v>22</v>
       </c>
       <c r="G9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" t="s">
         <v>43</v>
       </c>
       <c r="I9" t="s">
         <v>44</v>
       </c>
-      <c r="J9" t="s">
-        <v>45</v>
+      <c r="J9">
+        <v>0</v>
       </c>
       <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F10" t="s">
         <v>22</v>
       </c>
       <c r="G10" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I10" t="s">
         <v>62</v>
       </c>
-      <c r="I10" t="s">
-        <v>58</v>
-      </c>
-      <c r="J10" t="s">
-        <v>63</v>
+      <c r="J10">
+        <v>0</v>
       </c>
       <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L10" xr:uid="{F761CE15-AF34-4E73-B732-AD7C7249D5C1}"/>
+  <autoFilter ref="A1:K10" xr:uid="{F761CE15-AF34-4E73-B732-AD7C7249D5C1}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1835,7 +1829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M13" sqref="M13"/>
     </sheetView>
@@ -1855,46 +1849,46 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="N1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -1905,7 +1899,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1923,22 +1917,22 @@
         <v>2.78</v>
       </c>
       <c r="I2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J2">
         <v>48</v>
       </c>
       <c r="K2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1949,7 +1943,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -1967,19 +1961,19 @@
         <v>3.66</v>
       </c>
       <c r="I3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J3">
         <v>30</v>
       </c>
       <c r="L3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1990,7 +1984,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -2008,7 +2002,7 @@
         <v>5.4</v>
       </c>
       <c r="I4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J4">
         <v>28</v>
@@ -2018,10 +2012,10 @@
         <v>202,202,202</v>
       </c>
       <c r="M4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -2032,7 +2026,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -2050,25 +2044,25 @@
         <v>4.6500000000000004</v>
       </c>
       <c r="I5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J5">
         <v>28</v>
       </c>
       <c r="K5" t="s">
+        <v>101</v>
+      </c>
+      <c r="L5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M5" t="s">
+        <v>91</v>
+      </c>
+      <c r="N5" t="s">
+        <v>104</v>
+      </c>
+      <c r="O5" t="s">
         <v>102</v>
-      </c>
-      <c r="L5" t="s">
-        <v>77</v>
-      </c>
-      <c r="M5" t="s">
-        <v>92</v>
-      </c>
-      <c r="N5" t="s">
-        <v>105</v>
-      </c>
-      <c r="O5" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -2079,7 +2073,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -2097,19 +2091,19 @@
         <v>0.2</v>
       </c>
       <c r="I6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J6">
         <v>30</v>
       </c>
       <c r="L6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -2120,7 +2114,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -2138,16 +2132,16 @@
         <v>1.55</v>
       </c>
       <c r="I7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J7">
         <v>20</v>
       </c>
       <c r="M7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -2158,7 +2152,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2176,25 +2170,25 @@
         <v>0.2</v>
       </c>
       <c r="I8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J8">
         <v>30</v>
       </c>
       <c r="K8" t="s">
+        <v>101</v>
+      </c>
+      <c r="L8" t="s">
+        <v>76</v>
+      </c>
+      <c r="M8" t="s">
+        <v>91</v>
+      </c>
+      <c r="N8" t="s">
+        <v>107</v>
+      </c>
+      <c r="O8" t="s">
         <v>102</v>
-      </c>
-      <c r="L8" t="s">
-        <v>77</v>
-      </c>
-      <c r="M8" t="s">
-        <v>92</v>
-      </c>
-      <c r="N8" t="s">
-        <v>108</v>
-      </c>
-      <c r="O8" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -2205,7 +2199,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -2223,22 +2217,22 @@
         <v>0.79</v>
       </c>
       <c r="I9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J9">
         <v>18</v>
       </c>
       <c r="K9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -2249,7 +2243,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -2267,22 +2261,22 @@
         <v>0.79</v>
       </c>
       <c r="I10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J10">
         <v>18</v>
       </c>
       <c r="K10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -2293,7 +2287,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D11">
         <v>4</v>
@@ -2311,23 +2305,23 @@
         <v>6.78</v>
       </c>
       <c r="I11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J11">
         <v>14</v>
       </c>
       <c r="K11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L11" s="2" t="str">
         <f>"202,202,202"</f>
         <v>202,202,202</v>
       </c>
       <c r="M11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -2338,7 +2332,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -2356,25 +2350,25 @@
         <v>0.2</v>
       </c>
       <c r="I12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J12">
         <v>30</v>
       </c>
       <c r="K12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N12" t="s">
+        <v>113</v>
+      </c>
+      <c r="O12" t="s">
         <v>114</v>
-      </c>
-      <c r="O12" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2413,37 +2407,37 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" t="s">
         <v>65</v>
       </c>
-      <c r="D1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>66</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>67</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>68</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>69</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>70</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>71</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>72</v>
-      </c>
-      <c r="L1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2454,13 +2448,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F2">
         <v>0.2</v>
@@ -2475,13 +2469,13 @@
         <v>0.71</v>
       </c>
       <c r="J2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K2">
         <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
POT configs completed. Code appears to be producing powerpoint correctly from them.
</commit_message>
<xml_diff>
--- a/graph_configs.xlsx
+++ b/graph_configs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WNF\Documents\GIT PROJECTS\CWIS-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8796452-B1F6-48E0-BACA-7126FE0B4C35}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467EF872-460B-4E4C-8244-B2A8B253C895}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="7710" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="7710" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
   </bookViews>
   <sheets>
     <sheet name="slide.types" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="136">
   <si>
     <t>slide.type.id</t>
   </si>
@@ -376,10 +376,73 @@
     <t>49,49,38</t>
   </si>
   <si>
-    <t>School Dashboard:</t>
-  </si>
-  <si>
-    <t>slides.df.h$school[i]</t>
+    <t>config.slide.i$school</t>
+  </si>
+  <si>
+    <t>slide.subtitle</t>
+  </si>
+  <si>
+    <t>section.title</t>
+  </si>
+  <si>
+    <t>section.subtitle.1</t>
+  </si>
+  <si>
+    <t>section.subtitle.2</t>
+  </si>
+  <si>
+    <t>Participation Change</t>
+  </si>
+  <si>
+    <t>District Overview</t>
+  </si>
+  <si>
+    <t>CWIS Participation:</t>
+  </si>
+  <si>
+    <t>CWIS Participation by School</t>
+  </si>
+  <si>
+    <t>Performance Change</t>
+  </si>
+  <si>
+    <t>config.slide.i$module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baseline through 2017-18 SY: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rates of Implementation: </t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Running Total</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Documented above are the percent of school respondents who answered that they use module practices. For some modules, 'use' is determined by reqported frequency (e.g. 'most of the time' or 'always'); in other modules, 'use' is determined through agreement (e.g. 'agree' or 'strongly agree'). Please see Green Reports for a list of complete prompts.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">School Dashboard: </t>
+  </si>
+  <si>
+    <t>Average Rates of Implementation</t>
+  </si>
+  <si>
+    <t>Diving Deeper Into Performance Change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementation Performance: </t>
   </si>
 </sst>
 </file>
@@ -1231,7 +1294,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,7 +1541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
@@ -1827,11 +1890,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2365,10 +2428,1272 @@
         <v>91</v>
       </c>
       <c r="N12" t="s">
+        <v>132</v>
+      </c>
+      <c r="O12" t="s">
         <v>113</v>
       </c>
-      <c r="O12" t="s">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>0.67</v>
+      </c>
+      <c r="F13">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G13">
+        <v>0.36</v>
+      </c>
+      <c r="H13">
+        <v>0.79</v>
+      </c>
+      <c r="I13" t="s">
+        <v>75</v>
+      </c>
+      <c r="J13">
+        <v>18</v>
+      </c>
+      <c r="K13" t="s">
+        <v>101</v>
+      </c>
+      <c r="L13" t="s">
+        <v>112</v>
+      </c>
+      <c r="M13" t="s">
+        <v>91</v>
+      </c>
+      <c r="N13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>0.67</v>
+      </c>
+      <c r="F14">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G14">
+        <v>5.08</v>
+      </c>
+      <c r="H14">
+        <v>0.79</v>
+      </c>
+      <c r="I14" t="s">
+        <v>75</v>
+      </c>
+      <c r="J14">
+        <v>18</v>
+      </c>
+      <c r="K14" t="s">
+        <v>101</v>
+      </c>
+      <c r="L14" t="s">
+        <v>112</v>
+      </c>
+      <c r="M14" t="s">
+        <v>91</v>
+      </c>
+      <c r="N14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>0.34</v>
+      </c>
+      <c r="F15">
+        <v>2.31</v>
+      </c>
+      <c r="G15">
+        <v>6.73</v>
+      </c>
+      <c r="H15">
+        <v>6.78</v>
+      </c>
+      <c r="I15" t="s">
+        <v>75</v>
+      </c>
+      <c r="J15">
+        <v>14</v>
+      </c>
+      <c r="K15" t="s">
+        <v>101</v>
+      </c>
+      <c r="L15" s="2" t="str">
+        <f>"202,202,202"</f>
+        <v>202,202,202</v>
+      </c>
+      <c r="M15" t="s">
+        <v>111</v>
+      </c>
+      <c r="O15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>7.76</v>
+      </c>
+      <c r="G16">
+        <v>1.25</v>
+      </c>
+      <c r="H16">
+        <v>2.58</v>
+      </c>
+      <c r="I16" t="s">
+        <v>75</v>
+      </c>
+      <c r="J16">
+        <v>48</v>
+      </c>
+      <c r="K16" t="s">
+        <v>101</v>
+      </c>
+      <c r="L16" s="2" t="str">
+        <f>"255,255,255"</f>
+        <v>255,255,255</v>
+      </c>
+      <c r="M16" t="s">
+        <v>91</v>
+      </c>
+      <c r="N16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>0.16</v>
+      </c>
+      <c r="F17">
+        <v>6.02</v>
+      </c>
+      <c r="G17">
+        <v>1.25</v>
+      </c>
+      <c r="H17">
+        <v>3.44</v>
+      </c>
+      <c r="I17" t="s">
+        <v>75</v>
+      </c>
+      <c r="J17">
+        <v>30</v>
+      </c>
+      <c r="K17" t="s">
+        <v>101</v>
+      </c>
+      <c r="L17" s="2" t="str">
+        <f>"255,255,255"</f>
+        <v>255,255,255</v>
+      </c>
+      <c r="M17" t="s">
+        <v>91</v>
+      </c>
+      <c r="N17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>117</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>7.76</v>
+      </c>
+      <c r="G18">
+        <v>1.25</v>
+      </c>
+      <c r="H18">
+        <v>4.05</v>
+      </c>
+      <c r="I18" t="s">
+        <v>75</v>
+      </c>
+      <c r="J18">
+        <v>30</v>
+      </c>
+      <c r="K18" t="s">
+        <v>101</v>
+      </c>
+      <c r="L18" s="2" t="str">
+        <f>"255,255,255"</f>
+        <v>255,255,255</v>
+      </c>
+      <c r="M18" t="s">
+        <v>91</v>
+      </c>
+      <c r="N18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>0.71</v>
+      </c>
+      <c r="F19">
+        <v>7.76</v>
+      </c>
+      <c r="G19">
+        <v>0.15</v>
+      </c>
+      <c r="H19">
+        <v>0.15</v>
+      </c>
+      <c r="I19" t="s">
+        <v>75</v>
+      </c>
+      <c r="J19">
+        <v>40</v>
+      </c>
+      <c r="K19" t="s">
+        <v>101</v>
+      </c>
+      <c r="L19" t="s">
+        <v>112</v>
+      </c>
+      <c r="M19" t="s">
+        <v>91</v>
+      </c>
+      <c r="N19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
         <v>114</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>0.67</v>
+      </c>
+      <c r="F20">
+        <v>7.76</v>
+      </c>
+      <c r="G20">
+        <v>0.15</v>
+      </c>
+      <c r="H20">
+        <v>0.74</v>
+      </c>
+      <c r="I20" t="s">
+        <v>75</v>
+      </c>
+      <c r="J20">
+        <v>28</v>
+      </c>
+      <c r="K20" t="s">
+        <v>101</v>
+      </c>
+      <c r="L20" s="2" t="str">
+        <f>"202,202,202"</f>
+        <v>202,202,202</v>
+      </c>
+      <c r="M20" t="s">
+        <v>91</v>
+      </c>
+      <c r="N20" t="s">
+        <v>104</v>
+      </c>
+      <c r="O20" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>0.34</v>
+      </c>
+      <c r="F21">
+        <v>2.31</v>
+      </c>
+      <c r="G21">
+        <v>6.73</v>
+      </c>
+      <c r="H21">
+        <v>6.78</v>
+      </c>
+      <c r="I21" t="s">
+        <v>75</v>
+      </c>
+      <c r="J21">
+        <v>14</v>
+      </c>
+      <c r="K21" t="s">
+        <v>101</v>
+      </c>
+      <c r="L21" s="2" t="str">
+        <f>"202,202,202"</f>
+        <v>202,202,202</v>
+      </c>
+      <c r="M21" t="s">
+        <v>111</v>
+      </c>
+      <c r="O21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>0.34</v>
+      </c>
+      <c r="F22">
+        <v>2.31</v>
+      </c>
+      <c r="G22">
+        <v>6.73</v>
+      </c>
+      <c r="H22">
+        <v>6.78</v>
+      </c>
+      <c r="I22" t="s">
+        <v>75</v>
+      </c>
+      <c r="J22">
+        <v>14</v>
+      </c>
+      <c r="K22" t="s">
+        <v>101</v>
+      </c>
+      <c r="L22" s="2" t="str">
+        <f>"202,202,202"</f>
+        <v>202,202,202</v>
+      </c>
+      <c r="M22" t="s">
+        <v>111</v>
+      </c>
+      <c r="O22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>9</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0.71</v>
+      </c>
+      <c r="F23">
+        <v>7.76</v>
+      </c>
+      <c r="G23">
+        <v>0.15</v>
+      </c>
+      <c r="H23">
+        <v>0.15</v>
+      </c>
+      <c r="I23" t="s">
+        <v>75</v>
+      </c>
+      <c r="J23">
+        <v>40</v>
+      </c>
+      <c r="K23" t="s">
+        <v>101</v>
+      </c>
+      <c r="L23" t="s">
+        <v>112</v>
+      </c>
+      <c r="M23" t="s">
+        <v>91</v>
+      </c>
+      <c r="N23" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>4</v>
+      </c>
+      <c r="B24">
+        <v>24</v>
+      </c>
+      <c r="C24" t="s">
+        <v>115</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>7.76</v>
+      </c>
+      <c r="G24">
+        <v>1.25</v>
+      </c>
+      <c r="H24">
+        <v>2.58</v>
+      </c>
+      <c r="I24" t="s">
+        <v>75</v>
+      </c>
+      <c r="J24">
+        <v>48</v>
+      </c>
+      <c r="K24" t="s">
+        <v>101</v>
+      </c>
+      <c r="L24" s="2" t="str">
+        <f>"255,255,255"</f>
+        <v>255,255,255</v>
+      </c>
+      <c r="M24" t="s">
+        <v>91</v>
+      </c>
+      <c r="N24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25">
+        <v>25</v>
+      </c>
+      <c r="C25" t="s">
+        <v>116</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>0.16</v>
+      </c>
+      <c r="F25">
+        <v>6.02</v>
+      </c>
+      <c r="G25">
+        <v>1.25</v>
+      </c>
+      <c r="H25">
+        <v>3.44</v>
+      </c>
+      <c r="I25" t="s">
+        <v>75</v>
+      </c>
+      <c r="J25">
+        <v>30</v>
+      </c>
+      <c r="K25" t="s">
+        <v>101</v>
+      </c>
+      <c r="L25" s="2" t="str">
+        <f>"255,255,255"</f>
+        <v>255,255,255</v>
+      </c>
+      <c r="M25" t="s">
+        <v>91</v>
+      </c>
+      <c r="N25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <v>26</v>
+      </c>
+      <c r="C26" t="s">
+        <v>117</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>7.76</v>
+      </c>
+      <c r="G26">
+        <v>1.25</v>
+      </c>
+      <c r="H26">
+        <v>4.05</v>
+      </c>
+      <c r="I26" t="s">
+        <v>75</v>
+      </c>
+      <c r="J26">
+        <v>30</v>
+      </c>
+      <c r="K26" t="s">
+        <v>101</v>
+      </c>
+      <c r="L26" s="2" t="str">
+        <f>"255,255,255"</f>
+        <v>255,255,255</v>
+      </c>
+      <c r="M26" t="s">
+        <v>91</v>
+      </c>
+      <c r="N26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>11</v>
+      </c>
+      <c r="B27">
+        <v>27</v>
+      </c>
+      <c r="C27" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>0.71</v>
+      </c>
+      <c r="F27">
+        <v>7.76</v>
+      </c>
+      <c r="G27">
+        <v>0.15</v>
+      </c>
+      <c r="H27">
+        <v>0.15</v>
+      </c>
+      <c r="I27" t="s">
+        <v>75</v>
+      </c>
+      <c r="J27">
+        <v>40</v>
+      </c>
+      <c r="K27" t="s">
+        <v>101</v>
+      </c>
+      <c r="L27" t="s">
+        <v>112</v>
+      </c>
+      <c r="M27" t="s">
+        <v>91</v>
+      </c>
+      <c r="N27" t="s">
+        <v>125</v>
+      </c>
+      <c r="O27" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>11</v>
+      </c>
+      <c r="B28">
+        <v>28</v>
+      </c>
+      <c r="C28" t="s">
+        <v>114</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>0.67</v>
+      </c>
+      <c r="F28">
+        <v>7.76</v>
+      </c>
+      <c r="G28">
+        <v>0.15</v>
+      </c>
+      <c r="H28">
+        <v>0.74</v>
+      </c>
+      <c r="I28" t="s">
+        <v>75</v>
+      </c>
+      <c r="J28">
+        <v>28</v>
+      </c>
+      <c r="K28" t="s">
+        <v>101</v>
+      </c>
+      <c r="L28" s="2" t="str">
+        <f>"202,202,202"</f>
+        <v>202,202,202</v>
+      </c>
+      <c r="M28" t="s">
+        <v>91</v>
+      </c>
+      <c r="N28" t="s">
+        <v>124</v>
+      </c>
+      <c r="O28" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>11</v>
+      </c>
+      <c r="B29">
+        <v>29</v>
+      </c>
+      <c r="C29" t="s">
+        <v>110</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <v>0.34</v>
+      </c>
+      <c r="F29">
+        <v>2.31</v>
+      </c>
+      <c r="G29">
+        <v>6.73</v>
+      </c>
+      <c r="H29">
+        <v>6.78</v>
+      </c>
+      <c r="I29" t="s">
+        <v>75</v>
+      </c>
+      <c r="J29">
+        <v>14</v>
+      </c>
+      <c r="K29" t="s">
+        <v>101</v>
+      </c>
+      <c r="L29" s="2" t="str">
+        <f>"202,202,202"</f>
+        <v>202,202,202</v>
+      </c>
+      <c r="M29" t="s">
+        <v>111</v>
+      </c>
+      <c r="O29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>10</v>
+      </c>
+      <c r="B30">
+        <v>30</v>
+      </c>
+      <c r="C30" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>0.71</v>
+      </c>
+      <c r="F30">
+        <v>8.4700000000000006</v>
+      </c>
+      <c r="G30">
+        <v>0.15</v>
+      </c>
+      <c r="H30">
+        <v>0.15</v>
+      </c>
+      <c r="I30" t="s">
+        <v>75</v>
+      </c>
+      <c r="J30">
+        <v>40</v>
+      </c>
+      <c r="K30" t="s">
+        <v>101</v>
+      </c>
+      <c r="L30" t="s">
+        <v>112</v>
+      </c>
+      <c r="M30" t="s">
+        <v>91</v>
+      </c>
+      <c r="N30" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>10</v>
+      </c>
+      <c r="B31">
+        <v>31</v>
+      </c>
+      <c r="C31" t="s">
+        <v>114</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <v>0.67</v>
+      </c>
+      <c r="F31">
+        <v>7.76</v>
+      </c>
+      <c r="G31">
+        <v>0.15</v>
+      </c>
+      <c r="H31">
+        <v>0.74</v>
+      </c>
+      <c r="I31" t="s">
+        <v>75</v>
+      </c>
+      <c r="J31">
+        <v>28</v>
+      </c>
+      <c r="K31" t="s">
+        <v>101</v>
+      </c>
+      <c r="L31" s="2" t="str">
+        <f>"202,202,202"</f>
+        <v>202,202,202</v>
+      </c>
+      <c r="M31" t="s">
+        <v>91</v>
+      </c>
+      <c r="N31" t="s">
+        <v>124</v>
+      </c>
+      <c r="O31" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>10</v>
+      </c>
+      <c r="B32">
+        <v>32</v>
+      </c>
+      <c r="C32" t="s">
+        <v>110</v>
+      </c>
+      <c r="D32">
+        <v>3</v>
+      </c>
+      <c r="E32">
+        <v>0.34</v>
+      </c>
+      <c r="F32">
+        <v>2.31</v>
+      </c>
+      <c r="G32">
+        <v>6.73</v>
+      </c>
+      <c r="H32">
+        <v>6.78</v>
+      </c>
+      <c r="I32" t="s">
+        <v>75</v>
+      </c>
+      <c r="J32">
+        <v>14</v>
+      </c>
+      <c r="K32" t="s">
+        <v>101</v>
+      </c>
+      <c r="L32" s="2" t="str">
+        <f>"202,202,202"</f>
+        <v>202,202,202</v>
+      </c>
+      <c r="M32" t="s">
+        <v>111</v>
+      </c>
+      <c r="O32" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>10</v>
+      </c>
+      <c r="B33">
+        <v>33</v>
+      </c>
+      <c r="C33" t="s">
+        <v>130</v>
+      </c>
+      <c r="D33">
+        <v>4</v>
+      </c>
+      <c r="E33">
+        <v>1.05</v>
+      </c>
+      <c r="F33">
+        <v>8.4700000000000006</v>
+      </c>
+      <c r="G33">
+        <v>0.83</v>
+      </c>
+      <c r="H33">
+        <v>5.57</v>
+      </c>
+      <c r="I33" t="s">
+        <v>75</v>
+      </c>
+      <c r="J33">
+        <v>14</v>
+      </c>
+      <c r="L33" s="2" t="str">
+        <f>"202,202,202"</f>
+        <v>202,202,202</v>
+      </c>
+      <c r="M33" t="s">
+        <v>91</v>
+      </c>
+      <c r="N33" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>11</v>
+      </c>
+      <c r="B34">
+        <v>34</v>
+      </c>
+      <c r="C34" t="s">
+        <v>130</v>
+      </c>
+      <c r="D34">
+        <v>4</v>
+      </c>
+      <c r="E34">
+        <v>1.05</v>
+      </c>
+      <c r="F34">
+        <v>8.4700000000000006</v>
+      </c>
+      <c r="G34">
+        <v>0.83</v>
+      </c>
+      <c r="H34">
+        <v>5.57</v>
+      </c>
+      <c r="I34" t="s">
+        <v>75</v>
+      </c>
+      <c r="J34">
+        <v>14</v>
+      </c>
+      <c r="L34" s="2" t="str">
+        <f>"202,202,202"</f>
+        <v>202,202,202</v>
+      </c>
+      <c r="M34" t="s">
+        <v>91</v>
+      </c>
+      <c r="N34" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>5</v>
+      </c>
+      <c r="B35">
+        <v>35</v>
+      </c>
+      <c r="C35" t="s">
+        <v>115</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>7.76</v>
+      </c>
+      <c r="G35">
+        <v>1.25</v>
+      </c>
+      <c r="H35">
+        <v>2.58</v>
+      </c>
+      <c r="I35" t="s">
+        <v>75</v>
+      </c>
+      <c r="J35">
+        <v>48</v>
+      </c>
+      <c r="K35" t="s">
+        <v>101</v>
+      </c>
+      <c r="L35" s="2" t="str">
+        <f>"255,255,255"</f>
+        <v>255,255,255</v>
+      </c>
+      <c r="M35" t="s">
+        <v>91</v>
+      </c>
+      <c r="N35" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <v>36</v>
+      </c>
+      <c r="C36" t="s">
+        <v>116</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36">
+        <v>0.16</v>
+      </c>
+      <c r="F36">
+        <v>6.02</v>
+      </c>
+      <c r="G36">
+        <v>1.25</v>
+      </c>
+      <c r="H36">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I36" t="s">
+        <v>75</v>
+      </c>
+      <c r="J36">
+        <v>30</v>
+      </c>
+      <c r="K36" t="s">
+        <v>101</v>
+      </c>
+      <c r="L36" s="2" t="str">
+        <f>"255,255,255"</f>
+        <v>255,255,255</v>
+      </c>
+      <c r="M36" t="s">
+        <v>91</v>
+      </c>
+      <c r="N36" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>5</v>
+      </c>
+      <c r="B37">
+        <v>37</v>
+      </c>
+      <c r="C37" t="s">
+        <v>117</v>
+      </c>
+      <c r="D37">
+        <v>3</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>7.76</v>
+      </c>
+      <c r="G37">
+        <v>1.25</v>
+      </c>
+      <c r="H37">
+        <v>4.71</v>
+      </c>
+      <c r="I37" t="s">
+        <v>75</v>
+      </c>
+      <c r="J37">
+        <v>30</v>
+      </c>
+      <c r="K37" t="s">
+        <v>101</v>
+      </c>
+      <c r="L37" s="2" t="str">
+        <f>"255,255,255"</f>
+        <v>255,255,255</v>
+      </c>
+      <c r="M37" t="s">
+        <v>91</v>
+      </c>
+      <c r="O37" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>12</v>
+      </c>
+      <c r="B38">
+        <v>38</v>
+      </c>
+      <c r="C38" t="s">
+        <v>73</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>0.71</v>
+      </c>
+      <c r="F38">
+        <v>9.4600000000000009</v>
+      </c>
+      <c r="G38">
+        <v>0.15</v>
+      </c>
+      <c r="H38">
+        <v>0.15</v>
+      </c>
+      <c r="I38" t="s">
+        <v>75</v>
+      </c>
+      <c r="J38">
+        <v>40</v>
+      </c>
+      <c r="K38" t="s">
+        <v>101</v>
+      </c>
+      <c r="L38" t="s">
+        <v>112</v>
+      </c>
+      <c r="M38" t="s">
+        <v>91</v>
+      </c>
+      <c r="N38" t="s">
+        <v>135</v>
+      </c>
+      <c r="O38" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>12</v>
+      </c>
+      <c r="B39">
+        <v>39</v>
+      </c>
+      <c r="C39" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39">
+        <v>0.67</v>
+      </c>
+      <c r="F39">
+        <v>7.76</v>
+      </c>
+      <c r="G39">
+        <v>0.15</v>
+      </c>
+      <c r="H39">
+        <v>0.74</v>
+      </c>
+      <c r="I39" t="s">
+        <v>75</v>
+      </c>
+      <c r="J39">
+        <v>28</v>
+      </c>
+      <c r="K39" t="s">
+        <v>101</v>
+      </c>
+      <c r="L39" s="2" t="str">
+        <f>"202,202,202"</f>
+        <v>202,202,202</v>
+      </c>
+      <c r="M39" t="s">
+        <v>91</v>
+      </c>
+      <c r="O39" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>12</v>
+      </c>
+      <c r="B40">
+        <v>40</v>
+      </c>
+      <c r="C40" t="s">
+        <v>110</v>
+      </c>
+      <c r="D40">
+        <v>3</v>
+      </c>
+      <c r="E40">
+        <v>0.34</v>
+      </c>
+      <c r="F40">
+        <v>2.31</v>
+      </c>
+      <c r="G40">
+        <v>6.73</v>
+      </c>
+      <c r="H40">
+        <v>6.78</v>
+      </c>
+      <c r="I40" t="s">
+        <v>75</v>
+      </c>
+      <c r="J40">
+        <v>14</v>
+      </c>
+      <c r="K40" t="s">
+        <v>101</v>
+      </c>
+      <c r="L40" s="2" t="str">
+        <f>"202,202,202"</f>
+        <v>202,202,202</v>
+      </c>
+      <c r="M40" t="s">
+        <v>111</v>
+      </c>
+      <c r="O40" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Graphs and pot objects are now appearing on slides for one district. Will now test making presentations for all districts.
</commit_message>
<xml_diff>
--- a/graph_configs.xlsx
+++ b/graph_configs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WNF\Documents\GIT PROJECTS\CWIS-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467EF872-460B-4E4C-8244-B2A8B253C895}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA8B57F-077D-4A04-8E6F-E71B3174DB10}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="7710" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="7710" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
   </bookViews>
   <sheets>
     <sheet name="slide.types" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="slide.table.objects" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">graph.types!$A$1:$K$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">graph.types!$A$1:$O$10</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">slide.pot.objects!$A$1:$O$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">slide.types!$A$1:$F$13</definedName>
   </definedNames>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="135">
   <si>
     <t>slide.type.id</t>
   </si>
@@ -376,9 +376,6 @@
     <t>49,49,38</t>
   </si>
   <si>
-    <t>config.slide.i$school</t>
-  </si>
-  <si>
     <t>slide.subtitle</t>
   </si>
   <si>
@@ -406,27 +403,12 @@
     <t>Performance Change</t>
   </si>
   <si>
-    <t>config.slide.i$module</t>
-  </si>
-  <si>
     <t xml:space="preserve">Baseline through 2017-18 SY: </t>
   </si>
   <si>
     <t xml:space="preserve">Rates of Implementation: </t>
   </si>
   <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
@@ -443,6 +425,21 @@
   </si>
   <si>
     <t xml:space="preserve">Implementation Performance: </t>
+  </si>
+  <si>
+    <t>district participation by school level</t>
+  </si>
+  <si>
+    <t>district performance by school level</t>
+  </si>
+  <si>
+    <t>district performance by school level by module</t>
+  </si>
+  <si>
+    <t>config.slide.df.i$school</t>
+  </si>
+  <si>
+    <t>config.slide.df.i$module</t>
   </si>
 </sst>
 </file>
@@ -932,10 +929,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1539,55 +1537,74 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="46.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>130</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
@@ -1613,8 +1630,20 @@
       <c r="K2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <v>4.87</v>
+      </c>
+      <c r="M2">
+        <v>4.41</v>
+      </c>
+      <c r="N2">
+        <v>0.36</v>
+      </c>
+      <c r="O2">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -1648,8 +1677,20 @@
       <c r="K3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>4.87</v>
+      </c>
+      <c r="M3">
+        <v>4.41</v>
+      </c>
+      <c r="N3">
+        <v>0.36</v>
+      </c>
+      <c r="O3">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1680,8 +1721,20 @@
       <c r="K4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>4.87</v>
+      </c>
+      <c r="M4">
+        <v>4.41</v>
+      </c>
+      <c r="N4">
+        <v>5.08</v>
+      </c>
+      <c r="O4">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -1715,8 +1768,20 @@
       <c r="K5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>4.87</v>
+      </c>
+      <c r="M5">
+        <v>4.41</v>
+      </c>
+      <c r="N5">
+        <v>5.08</v>
+      </c>
+      <c r="O5">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1747,13 +1812,25 @@
       <c r="K6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="M6">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="N6">
+        <v>0.36</v>
+      </c>
+      <c r="O6">
+        <v>1.41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>130</v>
       </c>
       <c r="C7" t="s">
         <v>39</v>
@@ -1779,13 +1856,25 @@
       <c r="K7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>5.2</v>
+      </c>
+      <c r="M7">
+        <v>5.33</v>
+      </c>
+      <c r="N7">
+        <v>4.24</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>131</v>
       </c>
       <c r="C8" t="s">
         <v>58</v>
@@ -1811,13 +1900,25 @@
       <c r="K8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <v>4.13</v>
+      </c>
+      <c r="M8">
+        <v>8.1</v>
+      </c>
+      <c r="N8">
+        <v>0.83</v>
+      </c>
+      <c r="O8">
+        <v>1.31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>132</v>
       </c>
       <c r="C9" t="s">
         <v>58</v>
@@ -1846,8 +1947,20 @@
       <c r="K9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>4.13</v>
+      </c>
+      <c r="M9">
+        <v>8.1</v>
+      </c>
+      <c r="N9">
+        <v>0.83</v>
+      </c>
+      <c r="O9">
+        <v>1.31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1881,9 +1994,21 @@
       <c r="K10">
         <v>1</v>
       </c>
+      <c r="L10">
+        <v>4.68</v>
+      </c>
+      <c r="M10">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="N10">
+        <v>0.99</v>
+      </c>
+      <c r="O10">
+        <v>1.35</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K10" xr:uid="{F761CE15-AF34-4E73-B732-AD7C7249D5C1}"/>
+  <autoFilter ref="A1:O10" xr:uid="{9F70A23B-DE67-4A3E-AE25-1DB06C00BF95}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1892,9 +2017,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H38" sqref="H38"/>
+    <sheetView topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2428,10 +2553,10 @@
         <v>91</v>
       </c>
       <c r="N12" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="O12" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2575,7 +2700,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -2609,7 +2734,7 @@
         <v>91</v>
       </c>
       <c r="N16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -2620,7 +2745,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -2665,7 +2790,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D18">
         <v>3</v>
@@ -2699,7 +2824,7 @@
         <v>91</v>
       </c>
       <c r="N18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -2743,7 +2868,7 @@
         <v>91</v>
       </c>
       <c r="N19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -2754,7 +2879,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D20">
         <v>2</v>
@@ -2925,7 +3050,7 @@
         <v>91</v>
       </c>
       <c r="N23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -2936,7 +3061,7 @@
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -2970,7 +3095,7 @@
         <v>91</v>
       </c>
       <c r="N24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -2981,7 +3106,7 @@
         <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D25">
         <v>2</v>
@@ -3026,7 +3151,7 @@
         <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D26">
         <v>3</v>
@@ -3060,7 +3185,7 @@
         <v>91</v>
       </c>
       <c r="N26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -3104,10 +3229,10 @@
         <v>91</v>
       </c>
       <c r="N27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="O27" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -3118,7 +3243,7 @@
         <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D28">
         <v>2</v>
@@ -3152,7 +3277,7 @@
         <v>91</v>
       </c>
       <c r="N28" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="O28" t="s">
         <v>102</v>
@@ -3244,7 +3369,7 @@
         <v>91</v>
       </c>
       <c r="N30" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -3255,7 +3380,7 @@
         <v>31</v>
       </c>
       <c r="C31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D31">
         <v>2</v>
@@ -3289,7 +3414,7 @@
         <v>91</v>
       </c>
       <c r="N31" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="O31" t="s">
         <v>102</v>
@@ -3348,7 +3473,7 @@
         <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D33">
         <v>4</v>
@@ -3379,7 +3504,7 @@
         <v>91</v>
       </c>
       <c r="N33" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
@@ -3390,7 +3515,7 @@
         <v>34</v>
       </c>
       <c r="C34" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D34">
         <v>4</v>
@@ -3421,7 +3546,7 @@
         <v>91</v>
       </c>
       <c r="N34" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
@@ -3432,7 +3557,7 @@
         <v>35</v>
       </c>
       <c r="C35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -3466,7 +3591,7 @@
         <v>91</v>
       </c>
       <c r="N35" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
@@ -3477,7 +3602,7 @@
         <v>36</v>
       </c>
       <c r="C36" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D36">
         <v>2</v>
@@ -3522,7 +3647,7 @@
         <v>37</v>
       </c>
       <c r="C37" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D37">
         <v>3</v>
@@ -3556,7 +3681,7 @@
         <v>91</v>
       </c>
       <c r="O37" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
@@ -3600,10 +3725,10 @@
         <v>91</v>
       </c>
       <c r="N38" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="O38" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
@@ -3614,7 +3739,7 @@
         <v>39</v>
       </c>
       <c r="C39" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D39">
         <v>2</v>
@@ -3648,7 +3773,7 @@
         <v>91</v>
       </c>
       <c r="O39" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Appears to correctly create all slides and graphs for all districts!
Now on to multiple smaller tweaks & issues...
</commit_message>
<xml_diff>
--- a/graph_configs.xlsx
+++ b/graph_configs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WNF\Documents\GIT PROJECTS\CWIS-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA8B57F-077D-4A04-8E6F-E71B3174DB10}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A536A05-3F5C-426D-A4C5-A2942E711927}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="7710" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="7710" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
   </bookViews>
   <sheets>
     <sheet name="slide.types" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">graph.types!$A$1:$O$10</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">slide.pot.objects!$A$1:$O$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">slide.pot.objects!$A$1:$O$40</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">slide.types!$A$1:$F$13</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="136">
   <si>
     <t>slide.type.id</t>
   </si>
@@ -199,9 +199,6 @@
     <t>d</t>
   </si>
   <si>
-    <t>school performance by module</t>
-  </si>
-  <si>
     <t>district participation</t>
   </si>
   <si>
@@ -346,9 +343,6 @@
     <t>district.ids[h]</t>
   </si>
   <si>
-    <t>blah, blah, blah</t>
-  </si>
-  <si>
     <t xml:space="preserve">District: </t>
   </si>
   <si>
@@ -397,9 +391,6 @@
     <t>CWIS Participation:</t>
   </si>
   <si>
-    <t>CWIS Participation by School</t>
-  </si>
-  <si>
     <t>Performance Change</t>
   </si>
   <si>
@@ -440,6 +431,23 @@
   </si>
   <si>
     <t>config.slide.df.i$module</t>
+  </si>
+  <si>
+    <t>school level performance by module</t>
+  </si>
+  <si>
+    <t>CWIS Participation by School Level</t>
+  </si>
+  <si>
+    <t>This is a district report that will show aggregated data by school level as well as disaggregated data by building.
+The focus of this report is change from present status as compared to baseline for both CWIS participation, as well as implementation rates reported by educators.
+Implementation rates are presented as the rate of responses that marked either "most of the time" or "always" or "agree" or "strongly agree".
+Data are presented for five major activities: 1) Effective Teaching and Learning Practices, 2) Common Formative Assessment, 3) Data-based Decision-making, 4) Leadership, and, 5) Professional Development.
+State averages are presented for district aggregate charts, while district averages are presented on visuals for individual schools.
+Charts detailing implementation performance later in this report are presented "by response" so that the relative change in participation is also perceptible.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Report Version: </t>
   </si>
 </sst>
 </file>
@@ -929,11 +937,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1315,7 +1324,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -1335,7 +1344,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1349,7 +1358,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1363,7 +1372,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
@@ -1380,7 +1389,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -1400,7 +1409,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1414,7 +1423,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F7" t="s">
         <v>16</v>
@@ -1431,7 +1440,7 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F8" t="s">
         <v>18</v>
@@ -1448,7 +1457,7 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1462,7 +1471,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F10" t="s">
         <v>20</v>
@@ -1479,7 +1488,7 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E11" t="s">
         <v>22</v>
@@ -1499,7 +1508,7 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1516,7 +1525,7 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E13" t="s">
         <v>25</v>
@@ -1539,9 +1548,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
+      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1587,16 +1596,16 @@
         <v>37</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -1604,7 +1613,7 @@
         <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
@@ -1739,7 +1748,7 @@
         <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>132</v>
       </c>
       <c r="C5" t="s">
         <v>39</v>
@@ -1786,7 +1795,7 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
         <v>39</v>
@@ -1798,13 +1807,13 @@
         <v>41</v>
       </c>
       <c r="G6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" t="s">
         <v>56</v>
       </c>
-      <c r="H6" t="s">
-        <v>57</v>
-      </c>
       <c r="I6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -1830,7 +1839,7 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C7" t="s">
         <v>39</v>
@@ -1857,13 +1866,13 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>5.2</v>
+        <v>4.6900000000000004</v>
       </c>
       <c r="M7">
-        <v>5.33</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="N7">
-        <v>4.24</v>
+        <v>0.36</v>
       </c>
       <c r="O7">
         <v>1</v>
@@ -1874,10 +1883,10 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" t="s">
         <v>40</v>
@@ -1918,10 +1927,10 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D9" t="s">
         <v>40</v>
@@ -1965,28 +1974,28 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F10" t="s">
         <v>22</v>
       </c>
       <c r="G10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I10" t="s">
         <v>61</v>
-      </c>
-      <c r="H10" t="s">
-        <v>57</v>
-      </c>
-      <c r="I10" t="s">
-        <v>62</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -2017,9 +2026,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O39" sqref="O39"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2037,46 +2046,46 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="N1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -2087,7 +2096,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -2105,22 +2114,22 @@
         <v>2.78</v>
       </c>
       <c r="I2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J2">
         <v>48</v>
       </c>
       <c r="K2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -2131,7 +2140,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -2149,19 +2158,19 @@
         <v>3.66</v>
       </c>
       <c r="I3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J3">
         <v>30</v>
       </c>
       <c r="L3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -2172,7 +2181,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -2190,7 +2199,7 @@
         <v>5.4</v>
       </c>
       <c r="I4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J4">
         <v>28</v>
@@ -2200,10 +2209,13 @@
         <v>202,202,202</v>
       </c>
       <c r="M4" t="s">
-        <v>91</v>
+        <v>90</v>
+      </c>
+      <c r="N4" t="s">
+        <v>135</v>
       </c>
       <c r="O4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -2214,7 +2226,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -2232,25 +2244,25 @@
         <v>4.6500000000000004</v>
       </c>
       <c r="I5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J5">
         <v>28</v>
       </c>
       <c r="K5" t="s">
+        <v>100</v>
+      </c>
+      <c r="L5" t="s">
+        <v>75</v>
+      </c>
+      <c r="M5" t="s">
+        <v>90</v>
+      </c>
+      <c r="N5" t="s">
+        <v>102</v>
+      </c>
+      <c r="O5" t="s">
         <v>101</v>
-      </c>
-      <c r="L5" t="s">
-        <v>76</v>
-      </c>
-      <c r="M5" t="s">
-        <v>91</v>
-      </c>
-      <c r="N5" t="s">
-        <v>104</v>
-      </c>
-      <c r="O5" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -2261,7 +2273,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -2279,19 +2291,19 @@
         <v>0.2</v>
       </c>
       <c r="I6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J6">
         <v>30</v>
       </c>
       <c r="L6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -2302,7 +2314,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -2320,16 +2332,16 @@
         <v>1.55</v>
       </c>
       <c r="I7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J7">
         <v>20</v>
       </c>
       <c r="M7" t="s">
-        <v>91</v>
-      </c>
-      <c r="N7" t="s">
-        <v>103</v>
+        <v>90</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -2340,7 +2352,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2358,25 +2370,25 @@
         <v>0.2</v>
       </c>
       <c r="I8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J8">
         <v>30</v>
       </c>
       <c r="K8" t="s">
+        <v>100</v>
+      </c>
+      <c r="L8" t="s">
+        <v>75</v>
+      </c>
+      <c r="M8" t="s">
+        <v>90</v>
+      </c>
+      <c r="N8" t="s">
+        <v>105</v>
+      </c>
+      <c r="O8" t="s">
         <v>101</v>
-      </c>
-      <c r="L8" t="s">
-        <v>76</v>
-      </c>
-      <c r="M8" t="s">
-        <v>91</v>
-      </c>
-      <c r="N8" t="s">
-        <v>107</v>
-      </c>
-      <c r="O8" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -2387,7 +2399,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -2405,22 +2417,22 @@
         <v>0.79</v>
       </c>
       <c r="I9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J9">
         <v>18</v>
       </c>
       <c r="K9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -2431,7 +2443,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -2449,22 +2461,22 @@
         <v>0.79</v>
       </c>
       <c r="I10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J10">
         <v>18</v>
       </c>
       <c r="K10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -2475,7 +2487,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D11">
         <v>4</v>
@@ -2493,23 +2505,23 @@
         <v>6.78</v>
       </c>
       <c r="I11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J11">
         <v>14</v>
       </c>
       <c r="K11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L11" s="2" t="str">
         <f>"202,202,202"</f>
         <v>202,202,202</v>
       </c>
       <c r="M11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -2520,7 +2532,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -2538,25 +2550,25 @@
         <v>0.2</v>
       </c>
       <c r="I12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J12">
         <v>30</v>
       </c>
       <c r="K12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N12" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="O12" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2567,7 +2579,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -2585,22 +2597,22 @@
         <v>0.79</v>
       </c>
       <c r="I13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J13">
         <v>18</v>
       </c>
       <c r="K13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -2611,7 +2623,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D14">
         <v>3</v>
@@ -2629,22 +2641,22 @@
         <v>0.79</v>
       </c>
       <c r="I14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J14">
         <v>18</v>
       </c>
       <c r="K14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -2655,7 +2667,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D15">
         <v>4</v>
@@ -2673,23 +2685,23 @@
         <v>6.78</v>
       </c>
       <c r="I15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J15">
         <v>14</v>
       </c>
       <c r="K15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L15" s="2" t="str">
         <f>"202,202,202"</f>
         <v>202,202,202</v>
       </c>
       <c r="M15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -2700,7 +2712,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -2718,23 +2730,23 @@
         <v>2.58</v>
       </c>
       <c r="I16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J16">
         <v>48</v>
       </c>
       <c r="K16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L16" s="2" t="str">
         <f>"255,255,255"</f>
         <v>255,255,255</v>
       </c>
       <c r="M16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N16" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -2745,7 +2757,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -2763,23 +2775,23 @@
         <v>3.44</v>
       </c>
       <c r="I17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J17">
         <v>30</v>
       </c>
       <c r="K17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L17" s="2" t="str">
         <f>"255,255,255"</f>
         <v>255,255,255</v>
       </c>
       <c r="M17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -2790,7 +2802,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D18">
         <v>3</v>
@@ -2808,23 +2820,23 @@
         <v>4.05</v>
       </c>
       <c r="I18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J18">
         <v>30</v>
       </c>
       <c r="K18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L18" s="2" t="str">
         <f>"255,255,255"</f>
         <v>255,255,255</v>
       </c>
       <c r="M18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N18" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -2835,7 +2847,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -2853,22 +2865,22 @@
         <v>0.15</v>
       </c>
       <c r="I19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J19">
         <v>40</v>
       </c>
       <c r="K19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L19" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -2879,7 +2891,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D20">
         <v>2</v>
@@ -2897,26 +2909,26 @@
         <v>0.74</v>
       </c>
       <c r="I20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J20">
         <v>28</v>
       </c>
       <c r="K20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L20" s="2" t="str">
         <f>"202,202,202"</f>
         <v>202,202,202</v>
       </c>
       <c r="M20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N20" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -2927,7 +2939,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D21">
         <v>3</v>
@@ -2945,23 +2957,23 @@
         <v>6.78</v>
       </c>
       <c r="I21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J21">
         <v>14</v>
       </c>
       <c r="K21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L21" s="2" t="str">
         <f>"202,202,202"</f>
         <v>202,202,202</v>
       </c>
       <c r="M21" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -2972,7 +2984,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D22">
         <v>3</v>
@@ -2990,23 +3002,23 @@
         <v>6.78</v>
       </c>
       <c r="I22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J22">
         <v>14</v>
       </c>
       <c r="K22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L22" s="2" t="str">
         <f>"202,202,202"</f>
         <v>202,202,202</v>
       </c>
       <c r="M22" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -3017,7 +3029,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -3035,22 +3047,22 @@
         <v>0.15</v>
       </c>
       <c r="I23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J23">
         <v>40</v>
       </c>
       <c r="K23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L23" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N23" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -3061,7 +3073,7 @@
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -3079,23 +3091,23 @@
         <v>2.58</v>
       </c>
       <c r="I24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J24">
         <v>48</v>
       </c>
       <c r="K24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L24" s="2" t="str">
         <f>"255,255,255"</f>
         <v>255,255,255</v>
       </c>
       <c r="M24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N24" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -3106,7 +3118,7 @@
         <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D25">
         <v>2</v>
@@ -3124,23 +3136,23 @@
         <v>3.44</v>
       </c>
       <c r="I25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J25">
         <v>30</v>
       </c>
       <c r="K25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L25" s="2" t="str">
         <f>"255,255,255"</f>
         <v>255,255,255</v>
       </c>
       <c r="M25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -3151,7 +3163,7 @@
         <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D26">
         <v>3</v>
@@ -3169,23 +3181,23 @@
         <v>4.05</v>
       </c>
       <c r="I26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J26">
         <v>30</v>
       </c>
       <c r="K26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L26" s="2" t="str">
         <f>"255,255,255"</f>
         <v>255,255,255</v>
       </c>
       <c r="M26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N26" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -3196,7 +3208,7 @@
         <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -3214,25 +3226,25 @@
         <v>0.15</v>
       </c>
       <c r="I27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J27">
         <v>40</v>
       </c>
       <c r="K27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N27" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="O27" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -3243,7 +3255,7 @@
         <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D28">
         <v>2</v>
@@ -3252,7 +3264,7 @@
         <v>0.67</v>
       </c>
       <c r="F28">
-        <v>7.76</v>
+        <v>9.15</v>
       </c>
       <c r="G28">
         <v>0.15</v>
@@ -3261,26 +3273,26 @@
         <v>0.74</v>
       </c>
       <c r="I28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J28">
         <v>28</v>
       </c>
       <c r="K28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L28" s="2" t="str">
         <f>"202,202,202"</f>
         <v>202,202,202</v>
       </c>
       <c r="M28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N28" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="O28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -3291,7 +3303,7 @@
         <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D29">
         <v>3</v>
@@ -3309,23 +3321,23 @@
         <v>6.78</v>
       </c>
       <c r="I29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J29">
         <v>14</v>
       </c>
       <c r="K29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L29" s="2" t="str">
         <f>"202,202,202"</f>
         <v>202,202,202</v>
       </c>
       <c r="M29" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -3336,7 +3348,7 @@
         <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -3354,22 +3366,22 @@
         <v>0.15</v>
       </c>
       <c r="I30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J30">
         <v>40</v>
       </c>
       <c r="K30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L30" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N30" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -3380,7 +3392,7 @@
         <v>31</v>
       </c>
       <c r="C31" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D31">
         <v>2</v>
@@ -3389,7 +3401,7 @@
         <v>0.67</v>
       </c>
       <c r="F31">
-        <v>7.76</v>
+        <v>9.15</v>
       </c>
       <c r="G31">
         <v>0.15</v>
@@ -3398,26 +3410,26 @@
         <v>0.74</v>
       </c>
       <c r="I31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J31">
         <v>28</v>
       </c>
       <c r="K31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L31" s="2" t="str">
         <f>"202,202,202"</f>
         <v>202,202,202</v>
       </c>
       <c r="M31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N31" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="O31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -3428,7 +3440,7 @@
         <v>32</v>
       </c>
       <c r="C32" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D32">
         <v>3</v>
@@ -3446,23 +3458,23 @@
         <v>6.78</v>
       </c>
       <c r="I32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J32">
         <v>14</v>
       </c>
       <c r="K32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L32" s="2" t="str">
         <f>"202,202,202"</f>
         <v>202,202,202</v>
       </c>
       <c r="M32" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -3473,7 +3485,7 @@
         <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D33">
         <v>4</v>
@@ -3491,7 +3503,7 @@
         <v>5.57</v>
       </c>
       <c r="I33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J33">
         <v>14</v>
@@ -3501,10 +3513,10 @@
         <v>202,202,202</v>
       </c>
       <c r="M33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N33" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
@@ -3515,7 +3527,7 @@
         <v>34</v>
       </c>
       <c r="C34" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D34">
         <v>4</v>
@@ -3533,7 +3545,7 @@
         <v>5.57</v>
       </c>
       <c r="I34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J34">
         <v>14</v>
@@ -3543,10 +3555,10 @@
         <v>202,202,202</v>
       </c>
       <c r="M34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N34" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
@@ -3557,7 +3569,7 @@
         <v>35</v>
       </c>
       <c r="C35" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -3575,23 +3587,23 @@
         <v>2.58</v>
       </c>
       <c r="I35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J35">
         <v>48</v>
       </c>
       <c r="K35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L35" s="2" t="str">
         <f>"255,255,255"</f>
         <v>255,255,255</v>
       </c>
       <c r="M35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N35" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
@@ -3602,7 +3614,7 @@
         <v>36</v>
       </c>
       <c r="C36" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D36">
         <v>2</v>
@@ -3620,23 +3632,23 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="I36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J36">
         <v>30</v>
       </c>
       <c r="K36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L36" s="2" t="str">
         <f>"255,255,255"</f>
         <v>255,255,255</v>
       </c>
       <c r="M36" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
@@ -3647,7 +3659,7 @@
         <v>37</v>
       </c>
       <c r="C37" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D37">
         <v>3</v>
@@ -3665,23 +3677,23 @@
         <v>4.71</v>
       </c>
       <c r="I37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J37">
         <v>30</v>
       </c>
       <c r="K37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L37" s="2" t="str">
         <f>"255,255,255"</f>
         <v>255,255,255</v>
       </c>
       <c r="M37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O37" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
@@ -3692,7 +3704,7 @@
         <v>38</v>
       </c>
       <c r="C38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -3710,25 +3722,25 @@
         <v>0.15</v>
       </c>
       <c r="I38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J38">
         <v>40</v>
       </c>
       <c r="K38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L38" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M38" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N38" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="O38" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
@@ -3739,7 +3751,7 @@
         <v>39</v>
       </c>
       <c r="C39" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D39">
         <v>2</v>
@@ -3757,23 +3769,23 @@
         <v>0.74</v>
       </c>
       <c r="I39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J39">
         <v>28</v>
       </c>
       <c r="K39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L39" s="2" t="str">
         <f>"202,202,202"</f>
         <v>202,202,202</v>
       </c>
       <c r="M39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O39" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
@@ -3784,7 +3796,7 @@
         <v>40</v>
       </c>
       <c r="C40" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D40">
         <v>3</v>
@@ -3802,27 +3814,27 @@
         <v>6.78</v>
       </c>
       <c r="I40" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J40">
         <v>14</v>
       </c>
       <c r="K40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L40" s="2" t="str">
         <f>"202,202,202"</f>
         <v>202,202,202</v>
       </c>
       <c r="M40" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O40" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O6" xr:uid="{AAFC98FD-2B31-46F6-BF19-8C5861C2C493}">
+  <autoFilter ref="A1:O40" xr:uid="{AAFC98FD-2B31-46F6-BF19-8C5861C2C493}">
     <sortState ref="A2:O6">
       <sortCondition ref="B1:B5"/>
     </sortState>
@@ -3857,37 +3869,37 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
         <v>64</v>
       </c>
-      <c r="D1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>65</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>66</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>67</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>68</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>69</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>70</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>71</v>
-      </c>
-      <c r="L1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -3898,13 +3910,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F2">
         <v>0.2</v>
@@ -3919,13 +3931,13 @@
         <v>0.71</v>
       </c>
       <c r="J2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K2">
         <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating graphs. Solved some smaller formatting issues.
</commit_message>
<xml_diff>
--- a/graph_configs.xlsx
+++ b/graph_configs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WNF\Documents\GIT PROJECTS\CWIS-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A536A05-3F5C-426D-A4C5-A2942E711927}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557AFD0A-7A9A-420D-809D-C8B7D4362E1B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="7710" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
   </bookViews>
@@ -2028,7 +2028,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N5" sqref="N5"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2105,7 +2105,7 @@
         <v>0.85</v>
       </c>
       <c r="F2">
-        <v>7.76</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="G2">
         <v>1.27</v>
@@ -2149,7 +2149,7 @@
         <v>0.61</v>
       </c>
       <c r="F3">
-        <v>7.76</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="G3">
         <v>1.27</v>
@@ -2190,7 +2190,7 @@
         <v>0.67</v>
       </c>
       <c r="F4">
-        <v>7.76</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="G4">
         <v>1.27</v>
@@ -2235,7 +2235,7 @@
         <v>0.67</v>
       </c>
       <c r="F5">
-        <v>7.76</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="G5">
         <v>1.27</v>
@@ -2335,7 +2335,7 @@
         <v>74</v>
       </c>
       <c r="J7">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="M7" t="s">
         <v>90</v>
@@ -2721,7 +2721,7 @@
         <v>1</v>
       </c>
       <c r="F16">
-        <v>7.76</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="G16">
         <v>1.25</v>
@@ -2811,7 +2811,7 @@
         <v>1</v>
       </c>
       <c r="F18">
-        <v>7.76</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="G18">
         <v>1.25</v>
@@ -2856,7 +2856,7 @@
         <v>0.71</v>
       </c>
       <c r="F19">
-        <v>7.76</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="G19">
         <v>0.15</v>
@@ -2900,7 +2900,7 @@
         <v>0.67</v>
       </c>
       <c r="F20">
-        <v>7.76</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="G20">
         <v>0.15</v>
@@ -3038,7 +3038,7 @@
         <v>0.71</v>
       </c>
       <c r="F23">
-        <v>7.76</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="G23">
         <v>0.15</v>
@@ -3082,7 +3082,7 @@
         <v>1</v>
       </c>
       <c r="F24">
-        <v>7.76</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="G24">
         <v>1.25</v>
@@ -3172,7 +3172,7 @@
         <v>1</v>
       </c>
       <c r="F26">
-        <v>7.76</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="G26">
         <v>1.25</v>
@@ -3217,7 +3217,7 @@
         <v>0.71</v>
       </c>
       <c r="F27">
-        <v>7.76</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="G27">
         <v>0.15</v>
@@ -3578,7 +3578,7 @@
         <v>1</v>
       </c>
       <c r="F35">
-        <v>7.76</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="G35">
         <v>1.25</v>
@@ -3668,7 +3668,7 @@
         <v>1</v>
       </c>
       <c r="F37">
-        <v>7.76</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="G37">
         <v>1.25</v>
@@ -3760,7 +3760,7 @@
         <v>0.67</v>
       </c>
       <c r="F39">
-        <v>7.76</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="G39">
         <v>0.15</v>

</xml_diff>

<commit_message>
Formatting for numbers in data labels.
</commit_message>
<xml_diff>
--- a/graph_configs.xlsx
+++ b/graph_configs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WNF\Documents\GIT PROJECTS\CWIS-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557AFD0A-7A9A-420D-809D-C8B7D4362E1B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DC93BF-15E9-426E-9504-9E60E0B50575}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="7710" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
   </bookViews>
@@ -1550,7 +1550,7 @@
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2027,8 +2027,8 @@
   <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3578,7 +3578,7 @@
         <v>1</v>
       </c>
       <c r="F35">
-        <v>9.1999999999999993</v>
+        <v>7.76</v>
       </c>
       <c r="G35">
         <v>1.25</v>

</xml_diff>

<commit_message>
Updates with response to Jason's comments. Fixed aesthetic changes, now need to deal with data & calculation concerns.
</commit_message>
<xml_diff>
--- a/graph_configs.xlsx
+++ b/graph_configs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WNF\Documents\GIT PROJECTS\CWIS-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DC93BF-15E9-426E-9504-9E60E0B50575}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB1B15B-E00B-4A8E-BC11-441B7AEFBACD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="7710" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="136">
   <si>
     <t>slide.type.id</t>
   </si>
@@ -2024,11 +2024,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F36" sqref="F36"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2122,8 +2123,9 @@
       <c r="K2" t="s">
         <v>100</v>
       </c>
-      <c r="L2" t="s">
-        <v>75</v>
+      <c r="L2" s="2" t="str">
+        <f t="shared" ref="L2:L3" si="0">"199,183,199"</f>
+        <v>199,183,199</v>
       </c>
       <c r="M2" t="s">
         <v>90</v>
@@ -2163,8 +2165,9 @@
       <c r="J3">
         <v>30</v>
       </c>
-      <c r="L3" t="s">
-        <v>75</v>
+      <c r="L3" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>199,183,199</v>
       </c>
       <c r="M3" t="s">
         <v>90</v>
@@ -2173,7 +2176,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2252,8 +2255,9 @@
       <c r="K5" t="s">
         <v>100</v>
       </c>
-      <c r="L5" t="s">
-        <v>75</v>
+      <c r="L5" s="2" t="str">
+        <f t="shared" ref="L5:L6" si="1">"199,183,199"</f>
+        <v>199,183,199</v>
       </c>
       <c r="M5" t="s">
         <v>90</v>
@@ -2296,8 +2300,9 @@
       <c r="J6">
         <v>30</v>
       </c>
-      <c r="L6" t="s">
-        <v>75</v>
+      <c r="L6" s="2" t="str">
+        <f>"199,183,199"</f>
+        <v>199,183,199</v>
       </c>
       <c r="M6" t="s">
         <v>90</v>
@@ -2306,7 +2311,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -2378,8 +2383,9 @@
       <c r="K8" t="s">
         <v>100</v>
       </c>
-      <c r="L8" t="s">
-        <v>75</v>
+      <c r="L8" s="2" t="str">
+        <f>"199,183,199"</f>
+        <v>199,183,199</v>
       </c>
       <c r="M8" t="s">
         <v>90</v>
@@ -2391,7 +2397,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -2435,7 +2441,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -2479,7 +2485,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
@@ -2558,8 +2564,9 @@
       <c r="K12" t="s">
         <v>100</v>
       </c>
-      <c r="L12" t="s">
-        <v>75</v>
+      <c r="L12" s="2" t="str">
+        <f>"199,183,199"</f>
+        <v>199,183,199</v>
       </c>
       <c r="M12" t="s">
         <v>90</v>
@@ -2571,7 +2578,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7</v>
       </c>
@@ -2615,7 +2622,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7</v>
       </c>
@@ -2659,7 +2666,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7</v>
       </c>
@@ -2704,7 +2711,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
@@ -2749,7 +2756,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
@@ -2794,7 +2801,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
       </c>
@@ -2873,8 +2880,9 @@
       <c r="K19" t="s">
         <v>100</v>
       </c>
-      <c r="L19" t="s">
-        <v>110</v>
+      <c r="L19" s="2" t="str">
+        <f t="shared" ref="L19:L20" si="2">"199,183,199"</f>
+        <v>199,183,199</v>
       </c>
       <c r="M19" t="s">
         <v>90</v>
@@ -2918,8 +2926,8 @@
         <v>100</v>
       </c>
       <c r="L20" s="2" t="str">
-        <f>"202,202,202"</f>
-        <v>202,202,202</v>
+        <f t="shared" si="2"/>
+        <v>199,183,199</v>
       </c>
       <c r="M20" t="s">
         <v>90</v>
@@ -2931,7 +2939,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>8</v>
       </c>
@@ -2976,7 +2984,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
@@ -3055,8 +3063,9 @@
       <c r="K23" t="s">
         <v>100</v>
       </c>
-      <c r="L23" t="s">
-        <v>110</v>
+      <c r="L23" s="2" t="str">
+        <f>"199,183,199"</f>
+        <v>199,183,199</v>
       </c>
       <c r="M23" t="s">
         <v>90</v>
@@ -3065,7 +3074,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>4</v>
       </c>
@@ -3110,7 +3119,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>4</v>
       </c>
@@ -3155,7 +3164,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>4</v>
       </c>
@@ -3234,8 +3243,9 @@
       <c r="K27" t="s">
         <v>100</v>
       </c>
-      <c r="L27" t="s">
-        <v>110</v>
+      <c r="L27" s="2" t="str">
+        <f t="shared" ref="L27:L28" si="3">"199,183,199"</f>
+        <v>199,183,199</v>
       </c>
       <c r="M27" t="s">
         <v>90</v>
@@ -3282,8 +3292,8 @@
         <v>100</v>
       </c>
       <c r="L28" s="2" t="str">
-        <f>"202,202,202"</f>
-        <v>202,202,202</v>
+        <f t="shared" si="3"/>
+        <v>199,183,199</v>
       </c>
       <c r="M28" t="s">
         <v>90</v>
@@ -3295,7 +3305,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>11</v>
       </c>
@@ -3374,8 +3384,9 @@
       <c r="K30" t="s">
         <v>100</v>
       </c>
-      <c r="L30" t="s">
-        <v>110</v>
+      <c r="L30" s="2" t="str">
+        <f t="shared" ref="L30:L31" si="4">"199,183,199"</f>
+        <v>199,183,199</v>
       </c>
       <c r="M30" t="s">
         <v>90</v>
@@ -3419,8 +3430,8 @@
         <v>100</v>
       </c>
       <c r="L31" s="2" t="str">
-        <f>"202,202,202"</f>
-        <v>202,202,202</v>
+        <f t="shared" si="4"/>
+        <v>199,183,199</v>
       </c>
       <c r="M31" t="s">
         <v>90</v>
@@ -3432,7 +3443,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>10</v>
       </c>
@@ -3477,7 +3488,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>10</v>
       </c>
@@ -3519,7 +3530,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>11</v>
       </c>
@@ -3561,7 +3572,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>5</v>
       </c>
@@ -3606,7 +3617,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>5</v>
       </c>
@@ -3651,7 +3662,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>5</v>
       </c>
@@ -3730,8 +3741,9 @@
       <c r="K38" t="s">
         <v>100</v>
       </c>
-      <c r="L38" t="s">
-        <v>110</v>
+      <c r="L38" s="2" t="str">
+        <f t="shared" ref="L38:L39" si="5">"199,183,199"</f>
+        <v>199,183,199</v>
       </c>
       <c r="M38" t="s">
         <v>90</v>
@@ -3778,8 +3790,8 @@
         <v>100</v>
       </c>
       <c r="L39" s="2" t="str">
-        <f>"202,202,202"</f>
-        <v>202,202,202</v>
+        <f t="shared" si="5"/>
+        <v>199,183,199</v>
       </c>
       <c r="M39" t="s">
         <v>90</v>
@@ -3788,7 +3800,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>12</v>
       </c>
@@ -3835,8 +3847,13 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:O40" xr:uid="{AAFC98FD-2B31-46F6-BF19-8C5861C2C493}">
-    <sortState ref="A2:O6">
-      <sortCondition ref="B1:B5"/>
+    <filterColumn colId="11">
+      <filters>
+        <filter val="199,183,199"/>
+      </filters>
+    </filterColumn>
+    <sortState ref="A6:O39">
+      <sortCondition ref="L1:L40"/>
     </sortState>
   </autoFilter>
   <sortState ref="A2:O6">

</xml_diff>

<commit_message>
Fixed a number of issues on Jason's latest list.
</commit_message>
<xml_diff>
--- a/graph_configs.xlsx
+++ b/graph_configs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WNF\Documents\GIT PROJECTS\CWIS-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB1B15B-E00B-4A8E-BC11-441B7AEFBACD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DFA084-F582-4349-9B96-9983F117CC7E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="7710" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="7710" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
   </bookViews>
   <sheets>
     <sheet name="slide.types" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="139">
   <si>
     <t>slide.type.id</t>
   </si>
@@ -394,18 +394,12 @@
     <t>Performance Change</t>
   </si>
   <si>
-    <t xml:space="preserve">Baseline through 2017-18 SY: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Rates of Implementation: </t>
   </si>
   <si>
     <t>notes</t>
   </si>
   <si>
-    <t>Documented above are the percent of school respondents who answered that they use module practices. For some modules, 'use' is determined by reqported frequency (e.g. 'most of the time' or 'always'); in other modules, 'use' is determined through agreement (e.g. 'agree' or 'strongly agree'). Please see Green Reports for a list of complete prompts.</t>
-  </si>
-  <si>
     <t xml:space="preserve">School Dashboard: </t>
   </si>
   <si>
@@ -439,15 +433,30 @@
     <t>CWIS Participation by School Level</t>
   </si>
   <si>
-    <t>This is a district report that will show aggregated data by school level as well as disaggregated data by building.
-The focus of this report is change from present status as compared to baseline for both CWIS participation, as well as implementation rates reported by educators.
-Implementation rates are presented as the rate of responses that marked either "most of the time" or "always" or "agree" or "strongly agree".
-Data are presented for five major activities: 1) Effective Teaching and Learning Practices, 2) Common Formative Assessment, 3) Data-based Decision-making, 4) Leadership, and, 5) Professional Development.
-State averages are presented for district aggregate charts, while district averages are presented on visuals for individual schools.
+    <t xml:space="preserve">Report Version: </t>
+  </si>
+  <si>
+    <t>96,51,86</t>
+  </si>
+  <si>
+    <t>Baseline through 2017-18</t>
+  </si>
+  <si>
+    <t>1. This is a district report that will show aggregated data by school level as well as disaggregated data by building.
+2. The focus of this report is change from present status as compared to baseline for both CWIS participation, as well as implementation rates reported by educators.
+3. Implementation rates are presented as the rate of responses that marked either "most of the time" or "always" or "agree" or "strongly agree".
+4. Data are presented for five major activities: 1) Effective Teaching and Learning Practices, 2) Common Formative Assessment, 3) Data-based Decision-making, 4) Leadership, and, 5) Professional Development.
+5. State averages are presented for district aggregate charts, while district averages are presented on visuals for individual schools.
 Charts detailing implementation performance later in this report are presented "by response" so that the relative change in participation is also perceptible.</t>
   </si>
   <si>
-    <t xml:space="preserve">Report Version: </t>
+    <t xml:space="preserve">Baseline through 2017-18: </t>
+  </si>
+  <si>
+    <t>Documented above are the percent of school respondents who answered that they use MMD practices. "For some essential functions, 'use' is determined by reported frequency (e.g. 'most of the time' or 'always'); for other functions, 'use' is determined through agreement (e.g. 'agree' or 'strongly agree'). Please see Green Reports for a list of complete prompts.</t>
+  </si>
+  <si>
+    <t>Documented above are the percent of school respondents who answered that they use MMD practices. For some essential functions, 'use' is determined by reported frequency (e.g. 'most of the time' or 'always'); for other functions, 'use' is determined through agreement (e.g. 'agree' or 'strongly agree'). Please see Green Reports for a list of complete prompts.</t>
   </si>
 </sst>
 </file>
@@ -1548,9 +1557,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1613,7 +1622,7 @@
         <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
@@ -1748,7 +1757,7 @@
         <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C5" t="s">
         <v>39</v>
@@ -1810,7 +1819,7 @@
         <v>55</v>
       </c>
       <c r="H6" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="I6" t="s">
         <v>55</v>
@@ -1839,7 +1848,7 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C7" t="s">
         <v>39</v>
@@ -1883,7 +1892,7 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C8" t="s">
         <v>57</v>
@@ -1927,7 +1936,7 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C9" t="s">
         <v>57</v>
@@ -2024,12 +2033,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
+      <selection pane="bottomLeft" activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2123,9 +2131,8 @@
       <c r="K2" t="s">
         <v>100</v>
       </c>
-      <c r="L2" s="2" t="str">
-        <f t="shared" ref="L2:L3" si="0">"199,183,199"</f>
-        <v>199,183,199</v>
+      <c r="L2" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="M2" t="s">
         <v>90</v>
@@ -2165,9 +2172,8 @@
       <c r="J3">
         <v>30</v>
       </c>
-      <c r="L3" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>199,183,199</v>
+      <c r="L3" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="M3" t="s">
         <v>90</v>
@@ -2176,7 +2182,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2208,14 +2214,14 @@
         <v>28</v>
       </c>
       <c r="L4" s="2" t="str">
-        <f>"202,202,202"</f>
-        <v>202,202,202</v>
+        <f>"230,230,230"</f>
+        <v>230,230,230</v>
       </c>
       <c r="M4" t="s">
         <v>90</v>
       </c>
       <c r="N4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="O4" t="s">
         <v>98</v>
@@ -2255,9 +2261,8 @@
       <c r="K5" t="s">
         <v>100</v>
       </c>
-      <c r="L5" s="2" t="str">
-        <f t="shared" ref="L5:L6" si="1">"199,183,199"</f>
-        <v>199,183,199</v>
+      <c r="L5" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="M5" t="s">
         <v>90</v>
@@ -2300,9 +2305,8 @@
       <c r="J6">
         <v>30</v>
       </c>
-      <c r="L6" s="2" t="str">
-        <f>"199,183,199"</f>
-        <v>199,183,199</v>
+      <c r="L6" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="M6" t="s">
         <v>90</v>
@@ -2311,7 +2315,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -2346,7 +2350,7 @@
         <v>90</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -2383,9 +2387,8 @@
       <c r="K8" t="s">
         <v>100</v>
       </c>
-      <c r="L8" s="2" t="str">
-        <f>"199,183,199"</f>
-        <v>199,183,199</v>
+      <c r="L8" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="M8" t="s">
         <v>90</v>
@@ -2397,7 +2400,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -2411,7 +2414,7 @@
         <v>2</v>
       </c>
       <c r="E9">
-        <v>0.67</v>
+        <v>0.33</v>
       </c>
       <c r="F9">
         <v>4.0999999999999996</v>
@@ -2420,7 +2423,7 @@
         <v>0.36</v>
       </c>
       <c r="H9">
-        <v>0.79</v>
+        <v>1.19</v>
       </c>
       <c r="I9" t="s">
         <v>74</v>
@@ -2441,7 +2444,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -2464,7 +2467,7 @@
         <v>5.08</v>
       </c>
       <c r="H10">
-        <v>0.79</v>
+        <v>1.19</v>
       </c>
       <c r="I10" t="s">
         <v>74</v>
@@ -2485,7 +2488,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
@@ -2564,21 +2567,20 @@
       <c r="K12" t="s">
         <v>100</v>
       </c>
-      <c r="L12" s="2" t="str">
-        <f>"199,183,199"</f>
-        <v>199,183,199</v>
+      <c r="L12" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="M12" t="s">
         <v>90</v>
       </c>
       <c r="N12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="O12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7</v>
       </c>
@@ -2601,7 +2603,7 @@
         <v>0.36</v>
       </c>
       <c r="H13">
-        <v>0.79</v>
+        <v>1.19</v>
       </c>
       <c r="I13" t="s">
         <v>74</v>
@@ -2622,7 +2624,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7</v>
       </c>
@@ -2645,7 +2647,7 @@
         <v>5.08</v>
       </c>
       <c r="H14">
-        <v>0.79</v>
+        <v>1.19</v>
       </c>
       <c r="I14" t="s">
         <v>74</v>
@@ -2666,7 +2668,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7</v>
       </c>
@@ -2711,7 +2713,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
@@ -2756,7 +2758,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
@@ -2798,10 +2800,10 @@
         <v>90</v>
       </c>
       <c r="N17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
       </c>
@@ -2880,9 +2882,8 @@
       <c r="K19" t="s">
         <v>100</v>
       </c>
-      <c r="L19" s="2" t="str">
-        <f t="shared" ref="L19:L20" si="2">"199,183,199"</f>
-        <v>199,183,199</v>
+      <c r="L19" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="M19" t="s">
         <v>90</v>
@@ -2925,9 +2926,8 @@
       <c r="K20" t="s">
         <v>100</v>
       </c>
-      <c r="L20" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>199,183,199</v>
+      <c r="L20" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="M20" t="s">
         <v>90</v>
@@ -2939,7 +2939,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>8</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
@@ -3063,18 +3063,17 @@
       <c r="K23" t="s">
         <v>100</v>
       </c>
-      <c r="L23" s="2" t="str">
-        <f>"199,183,199"</f>
-        <v>199,183,199</v>
+      <c r="L23" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="M23" t="s">
         <v>90</v>
       </c>
       <c r="N23" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>4</v>
       </c>
@@ -3119,7 +3118,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>4</v>
       </c>
@@ -3161,10 +3160,10 @@
         <v>90</v>
       </c>
       <c r="N25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>4</v>
       </c>
@@ -3243,18 +3242,17 @@
       <c r="K27" t="s">
         <v>100</v>
       </c>
-      <c r="L27" s="2" t="str">
-        <f t="shared" ref="L27:L28" si="3">"199,183,199"</f>
-        <v>199,183,199</v>
+      <c r="L27" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="M27" t="s">
         <v>90</v>
       </c>
       <c r="N27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O27" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -3291,21 +3289,20 @@
       <c r="K28" t="s">
         <v>100</v>
       </c>
-      <c r="L28" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>199,183,199</v>
+      <c r="L28" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="M28" t="s">
         <v>90</v>
       </c>
       <c r="N28" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="O28" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>11</v>
       </c>
@@ -3384,15 +3381,14 @@
       <c r="K30" t="s">
         <v>100</v>
       </c>
-      <c r="L30" s="2" t="str">
-        <f t="shared" ref="L30:L31" si="4">"199,183,199"</f>
-        <v>199,183,199</v>
+      <c r="L30" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="M30" t="s">
         <v>90</v>
       </c>
       <c r="N30" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -3429,21 +3425,20 @@
       <c r="K31" t="s">
         <v>100</v>
       </c>
-      <c r="L31" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>199,183,199</v>
+      <c r="L31" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="M31" t="s">
         <v>90</v>
       </c>
       <c r="N31" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="O31" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>10</v>
       </c>
@@ -3488,7 +3483,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>10</v>
       </c>
@@ -3496,7 +3491,7 @@
         <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D33">
         <v>4</v>
@@ -3527,10 +3522,10 @@
         <v>90</v>
       </c>
       <c r="N33" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>11</v>
       </c>
@@ -3538,7 +3533,7 @@
         <v>34</v>
       </c>
       <c r="C34" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D34">
         <v>4</v>
@@ -3569,10 +3564,10 @@
         <v>90</v>
       </c>
       <c r="N34" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>5</v>
       </c>
@@ -3614,10 +3609,10 @@
         <v>90</v>
       </c>
       <c r="N35" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>5</v>
       </c>
@@ -3659,10 +3654,10 @@
         <v>90</v>
       </c>
       <c r="N36" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>5</v>
       </c>
@@ -3704,7 +3699,7 @@
         <v>90</v>
       </c>
       <c r="O37" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
@@ -3741,18 +3736,17 @@
       <c r="K38" t="s">
         <v>100</v>
       </c>
-      <c r="L38" s="2" t="str">
-        <f t="shared" ref="L38:L39" si="5">"199,183,199"</f>
-        <v>199,183,199</v>
+      <c r="L38" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="M38" t="s">
         <v>90</v>
       </c>
       <c r="N38" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="O38" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
@@ -3789,18 +3783,17 @@
       <c r="K39" t="s">
         <v>100</v>
       </c>
-      <c r="L39" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>199,183,199</v>
+      <c r="L39" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="M39" t="s">
         <v>90</v>
       </c>
       <c r="O39" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>12</v>
       </c>
@@ -3846,16 +3839,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O40" xr:uid="{AAFC98FD-2B31-46F6-BF19-8C5861C2C493}">
-    <filterColumn colId="11">
-      <filters>
-        <filter val="199,183,199"/>
-      </filters>
-    </filterColumn>
-    <sortState ref="A6:O39">
-      <sortCondition ref="L1:L40"/>
-    </sortState>
-  </autoFilter>
   <sortState ref="A2:O6">
     <sortCondition ref="A2:A6"/>
     <sortCondition ref="D2:D6"/>

</xml_diff>

<commit_message>
Further fixing of small issues for Jason, slight reorganization of folders to clean out directory a little.
</commit_message>
<xml_diff>
--- a/graph_configs.xlsx
+++ b/graph_configs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WNF\Documents\GIT PROJECTS\CWIS-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DFA084-F582-4349-9B96-9983F117CC7E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1588C9F-D0C2-40F5-BBC8-D193019D042C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="7710" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="7710" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
   </bookViews>
   <sheets>
     <sheet name="slide.types" sheetId="1" r:id="rId1"/>
@@ -1557,9 +1557,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2035,9 +2035,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K14" sqref="K14"/>
+      <selection pane="bottomLeft" activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
- Added average labels as pot objects using config spreadsheet - Made graph labels white when over purple (very confusingly, one graph for district participation reverses them so had to add if-then statement)
</commit_message>
<xml_diff>
--- a/graph_configs.xlsx
+++ b/graph_configs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WNF\Documents\GIT PROJECTS\CWIS-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1588C9F-D0C2-40F5-BBC8-D193019D042C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB91CF4A-A761-4A9D-BDC4-73A66B949D6F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="7710" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">graph.types!$A$1:$O$10</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">slide.pot.objects!$A$1:$O$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">slide.pot.objects!$A$1:$O$48</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">slide.types!$A$1:$F$13</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="144">
   <si>
     <t>slide.type.id</t>
   </si>
@@ -457,6 +457,21 @@
   </si>
   <si>
     <t>Documented above are the percent of school respondents who answered that they use MMD practices. For some essential functions, 'use' is determined by reported frequency (e.g. 'most of the time' or 'always'); for other functions, 'use' is determined through agreement (e.g. 'agree' or 'strongly agree'). Please see Green Reports for a list of complete prompts.</t>
+  </si>
+  <si>
+    <t>average.legend.1</t>
+  </si>
+  <si>
+    <t>average.legend.2</t>
+  </si>
+  <si>
+    <t>l state average</t>
+  </si>
+  <si>
+    <t>0,0,0</t>
+  </si>
+  <si>
+    <t>l district average</t>
   </si>
 </sst>
 </file>
@@ -1310,7 +1325,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2033,11 +2048,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:O40"/>
+  <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2146,16 +2161,16 @@
         <v>1</v>
       </c>
       <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
       <c r="E3">
-        <v>0.61</v>
+        <v>0.67</v>
       </c>
       <c r="F3">
         <v>9.1999999999999993</v>
@@ -2164,22 +2179,26 @@
         <v>1.27</v>
       </c>
       <c r="H3">
-        <v>3.66</v>
+        <v>5.4</v>
       </c>
       <c r="I3" t="s">
         <v>74</v>
       </c>
       <c r="J3">
-        <v>30</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>133</v>
+        <v>28</v>
+      </c>
+      <c r="L3" s="2" t="str">
+        <f>"230,230,230"</f>
+        <v>230,230,230</v>
       </c>
       <c r="M3" t="s">
         <v>90</v>
       </c>
       <c r="N3" t="s">
-        <v>89</v>
+        <v>132</v>
+      </c>
+      <c r="O3" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -2187,13 +2206,13 @@
         <v>1</v>
       </c>
       <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4">
         <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
       </c>
       <c r="E4">
         <v>0.67</v>
@@ -2205,7 +2224,7 @@
         <v>1.27</v>
       </c>
       <c r="H4">
-        <v>5.4</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="I4" t="s">
         <v>74</v>
@@ -2213,18 +2232,20 @@
       <c r="J4">
         <v>28</v>
       </c>
-      <c r="L4" s="2" t="str">
-        <f>"230,230,230"</f>
-        <v>230,230,230</v>
+      <c r="K4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="M4" t="s">
         <v>90</v>
       </c>
       <c r="N4" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="O4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -2232,16 +2253,16 @@
         <v>1</v>
       </c>
       <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
       <c r="E5">
-        <v>0.67</v>
+        <v>0.61</v>
       </c>
       <c r="F5">
         <v>9.1999999999999993</v>
@@ -2250,16 +2271,13 @@
         <v>1.27</v>
       </c>
       <c r="H5">
-        <v>4.6500000000000004</v>
+        <v>3.66</v>
       </c>
       <c r="I5" t="s">
         <v>74</v>
       </c>
       <c r="J5">
-        <v>28</v>
-      </c>
-      <c r="K5" t="s">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>133</v>
@@ -2268,10 +2286,7 @@
         <v>90</v>
       </c>
       <c r="N5" t="s">
-        <v>102</v>
-      </c>
-      <c r="O5" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -2355,46 +2370,44 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E8">
-        <v>0.71</v>
+        <v>0.34</v>
       </c>
       <c r="F8">
-        <v>9.2100000000000009</v>
+        <v>2.31</v>
       </c>
       <c r="G8">
-        <v>0.28999999999999998</v>
+        <v>6.73</v>
       </c>
       <c r="H8">
-        <v>0.2</v>
+        <v>6.78</v>
       </c>
       <c r="I8" t="s">
         <v>74</v>
       </c>
       <c r="J8">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="K8" t="s">
         <v>100</v>
       </c>
-      <c r="L8" s="2" t="s">
-        <v>133</v>
+      <c r="L8" s="2" t="str">
+        <f>"202,202,202"</f>
+        <v>202,202,202</v>
       </c>
       <c r="M8" t="s">
-        <v>90</v>
-      </c>
-      <c r="N8" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="O8" t="s">
         <v>101</v>
@@ -2402,347 +2415,349 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>4.0999999999999996</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="G9">
-        <v>0.36</v>
+        <v>1.25</v>
       </c>
       <c r="H9">
-        <v>1.19</v>
+        <v>2.58</v>
       </c>
       <c r="I9" t="s">
         <v>74</v>
       </c>
       <c r="J9">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="K9" t="s">
         <v>100</v>
       </c>
-      <c r="L9" t="s">
-        <v>110</v>
+      <c r="L9" s="2" t="str">
+        <f>"255,255,255"</f>
+        <v>255,255,255</v>
       </c>
       <c r="M9" t="s">
         <v>90</v>
       </c>
       <c r="N9" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>0.67</v>
+        <v>0.16</v>
       </c>
       <c r="F10">
-        <v>4.0999999999999996</v>
+        <v>6.02</v>
       </c>
       <c r="G10">
-        <v>5.08</v>
+        <v>1.25</v>
       </c>
       <c r="H10">
-        <v>1.19</v>
+        <v>3.44</v>
       </c>
       <c r="I10" t="s">
         <v>74</v>
       </c>
       <c r="J10">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K10" t="s">
         <v>100</v>
       </c>
-      <c r="L10" t="s">
-        <v>110</v>
+      <c r="L10" s="2" t="str">
+        <f>"255,255,255"</f>
+        <v>255,255,255</v>
       </c>
       <c r="M10" t="s">
         <v>90</v>
       </c>
       <c r="N10" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E11">
-        <v>0.34</v>
+        <v>1</v>
       </c>
       <c r="F11">
-        <v>2.31</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="G11">
-        <v>6.73</v>
+        <v>1.25</v>
       </c>
       <c r="H11">
-        <v>6.78</v>
+        <v>4.05</v>
       </c>
       <c r="I11" t="s">
         <v>74</v>
       </c>
       <c r="J11">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="K11" t="s">
         <v>100</v>
       </c>
       <c r="L11" s="2" t="str">
-        <f>"202,202,202"</f>
-        <v>202,202,202</v>
+        <f>"255,255,255"</f>
+        <v>255,255,255</v>
       </c>
       <c r="M11" t="s">
-        <v>109</v>
-      </c>
-      <c r="O11" t="s">
-        <v>101</v>
+        <v>90</v>
+      </c>
+      <c r="N11" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>112</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12">
-        <v>0.71</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <v>9.2100000000000009</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="G12">
-        <v>0.28999999999999998</v>
+        <v>1.25</v>
       </c>
       <c r="H12">
-        <v>0.2</v>
+        <v>2.58</v>
       </c>
       <c r="I12" t="s">
         <v>74</v>
       </c>
       <c r="J12">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="K12" t="s">
         <v>100</v>
       </c>
-      <c r="L12" s="2" t="s">
-        <v>133</v>
+      <c r="L12" s="2" t="str">
+        <f>"255,255,255"</f>
+        <v>255,255,255</v>
       </c>
       <c r="M12" t="s">
         <v>90</v>
       </c>
       <c r="N12" t="s">
-        <v>121</v>
-      </c>
-      <c r="O12" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B13">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="D13">
         <v>2</v>
       </c>
       <c r="E13">
-        <v>0.67</v>
+        <v>0.16</v>
       </c>
       <c r="F13">
-        <v>4.0999999999999996</v>
+        <v>6.02</v>
       </c>
       <c r="G13">
-        <v>0.36</v>
+        <v>1.25</v>
       </c>
       <c r="H13">
-        <v>1.19</v>
+        <v>3.44</v>
       </c>
       <c r="I13" t="s">
         <v>74</v>
       </c>
       <c r="J13">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K13" t="s">
         <v>100</v>
       </c>
-      <c r="L13" t="s">
-        <v>110</v>
+      <c r="L13" s="2" t="str">
+        <f>"255,255,255"</f>
+        <v>255,255,255</v>
       </c>
       <c r="M13" t="s">
         <v>90</v>
       </c>
       <c r="N13" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B14">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="D14">
         <v>3</v>
       </c>
       <c r="E14">
-        <v>0.67</v>
+        <v>1</v>
       </c>
       <c r="F14">
-        <v>4.0999999999999996</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="G14">
-        <v>5.08</v>
+        <v>1.25</v>
       </c>
       <c r="H14">
-        <v>1.19</v>
+        <v>4.05</v>
       </c>
       <c r="I14" t="s">
         <v>74</v>
       </c>
       <c r="J14">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="K14" t="s">
         <v>100</v>
       </c>
-      <c r="L14" t="s">
-        <v>110</v>
+      <c r="L14" s="2" t="str">
+        <f>"255,255,255"</f>
+        <v>255,255,255</v>
       </c>
       <c r="M14" t="s">
         <v>90</v>
       </c>
       <c r="N14" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B15">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>0.34</v>
+        <v>1</v>
       </c>
       <c r="F15">
-        <v>2.31</v>
+        <v>7.76</v>
       </c>
       <c r="G15">
-        <v>6.73</v>
+        <v>1.25</v>
       </c>
       <c r="H15">
-        <v>6.78</v>
+        <v>2.58</v>
       </c>
       <c r="I15" t="s">
         <v>74</v>
       </c>
       <c r="J15">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="K15" t="s">
         <v>100</v>
       </c>
       <c r="L15" s="2" t="str">
-        <f>"202,202,202"</f>
-        <v>202,202,202</v>
+        <f>"255,255,255"</f>
+        <v>255,255,255</v>
       </c>
       <c r="M15" t="s">
-        <v>109</v>
-      </c>
-      <c r="O15" t="s">
-        <v>101</v>
+        <v>90</v>
+      </c>
+      <c r="N15" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B16">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>0.16</v>
       </c>
       <c r="F16">
-        <v>9.1999999999999993</v>
+        <v>6.02</v>
       </c>
       <c r="G16">
         <v>1.25</v>
       </c>
       <c r="H16">
-        <v>2.58</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="I16" t="s">
         <v>74</v>
       </c>
       <c r="J16">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="K16" t="s">
         <v>100</v>
@@ -2755,33 +2770,33 @@
         <v>90</v>
       </c>
       <c r="N16" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>37</v>
+      </c>
+      <c r="C17" t="s">
+        <v>114</v>
+      </c>
+      <c r="D17">
         <v>3</v>
       </c>
-      <c r="B17">
-        <v>16</v>
-      </c>
-      <c r="C17" t="s">
-        <v>113</v>
-      </c>
-      <c r="D17">
-        <v>2</v>
-      </c>
       <c r="E17">
-        <v>0.16</v>
+        <v>1</v>
       </c>
       <c r="F17">
-        <v>6.02</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="G17">
         <v>1.25</v>
       </c>
       <c r="H17">
-        <v>3.44</v>
+        <v>4.71</v>
       </c>
       <c r="I17" t="s">
         <v>74</v>
@@ -2799,34 +2814,34 @@
       <c r="M17" t="s">
         <v>90</v>
       </c>
-      <c r="N17" t="s">
-        <v>134</v>
+      <c r="O17" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B18">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>114</v>
+        <v>72</v>
       </c>
       <c r="D18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>0.71</v>
       </c>
       <c r="F18">
-        <v>9.1999999999999993</v>
+        <v>9.2100000000000009</v>
       </c>
       <c r="G18">
-        <v>1.25</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="H18">
-        <v>4.05</v>
+        <v>0.2</v>
       </c>
       <c r="I18" t="s">
         <v>74</v>
@@ -2837,120 +2852,119 @@
       <c r="K18" t="s">
         <v>100</v>
       </c>
-      <c r="L18" s="2" t="str">
-        <f>"255,255,255"</f>
-        <v>255,255,255</v>
+      <c r="L18" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="M18" t="s">
         <v>90</v>
       </c>
       <c r="N18" t="s">
-        <v>116</v>
+        <v>105</v>
+      </c>
+      <c r="O18" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19">
         <v>8</v>
       </c>
-      <c r="B19">
+      <c r="C19" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>0.33</v>
+      </c>
+      <c r="F19">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G19">
+        <v>0.36</v>
+      </c>
+      <c r="H19">
+        <v>1.19</v>
+      </c>
+      <c r="I19" t="s">
+        <v>74</v>
+      </c>
+      <c r="J19">
         <v>18</v>
-      </c>
-      <c r="C19" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>0.71</v>
-      </c>
-      <c r="F19">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="G19">
-        <v>0.15</v>
-      </c>
-      <c r="H19">
-        <v>0.15</v>
-      </c>
-      <c r="I19" t="s">
-        <v>74</v>
-      </c>
-      <c r="J19">
-        <v>40</v>
       </c>
       <c r="K19" t="s">
         <v>100</v>
       </c>
-      <c r="L19" s="2" t="s">
-        <v>133</v>
+      <c r="L19" t="s">
+        <v>110</v>
       </c>
       <c r="M19" t="s">
         <v>90</v>
       </c>
       <c r="N19" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B20">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E20">
         <v>0.67</v>
       </c>
       <c r="F20">
-        <v>9.1999999999999993</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="G20">
-        <v>0.15</v>
+        <v>5.08</v>
       </c>
       <c r="H20">
-        <v>0.74</v>
+        <v>1.19</v>
       </c>
       <c r="I20" t="s">
         <v>74</v>
       </c>
       <c r="J20">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="K20" t="s">
         <v>100</v>
       </c>
-      <c r="L20" s="2" t="s">
-        <v>133</v>
+      <c r="L20" t="s">
+        <v>110</v>
       </c>
       <c r="M20" t="s">
         <v>90</v>
       </c>
       <c r="N20" t="s">
-        <v>102</v>
-      </c>
-      <c r="O20" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B21">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C21" t="s">
         <v>108</v>
       </c>
       <c r="D21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E21">
         <v>0.34</v>
@@ -2986,373 +3000,354 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <v>41</v>
+      </c>
+      <c r="C22" t="s">
+        <v>139</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <v>0.3</v>
+      </c>
+      <c r="F22">
+        <v>1.19</v>
+      </c>
+      <c r="G22">
+        <v>0.87</v>
+      </c>
+      <c r="H22">
+        <v>1.67</v>
+      </c>
+      <c r="I22" t="s">
+        <v>74</v>
+      </c>
+      <c r="J22">
+        <v>12</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="M22" t="s">
+        <v>90</v>
+      </c>
+      <c r="N22" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>42</v>
+      </c>
+      <c r="C23" t="s">
+        <v>140</v>
+      </c>
+      <c r="D23">
+        <v>6</v>
+      </c>
+      <c r="E23">
+        <v>0.3</v>
+      </c>
+      <c r="F23">
+        <v>1.19</v>
+      </c>
+      <c r="G23">
+        <v>5.51</v>
+      </c>
+      <c r="H23">
+        <v>1.67</v>
+      </c>
+      <c r="I23" t="s">
+        <v>74</v>
+      </c>
+      <c r="J23">
+        <v>12</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="M23" t="s">
+        <v>90</v>
+      </c>
+      <c r="N23" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>7</v>
+      </c>
+      <c r="B24">
+        <v>11</v>
+      </c>
+      <c r="C24" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>0.71</v>
+      </c>
+      <c r="F24">
+        <v>9.2100000000000009</v>
+      </c>
+      <c r="G24">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H24">
+        <v>0.2</v>
+      </c>
+      <c r="I24" t="s">
+        <v>74</v>
+      </c>
+      <c r="J24">
+        <v>30</v>
+      </c>
+      <c r="K24" t="s">
+        <v>100</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="M24" t="s">
+        <v>90</v>
+      </c>
+      <c r="N24" t="s">
+        <v>121</v>
+      </c>
+      <c r="O24" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>7</v>
+      </c>
+      <c r="B25">
+        <v>12</v>
+      </c>
+      <c r="C25" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25">
         <v>2</v>
       </c>
-      <c r="B22">
-        <v>21</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="E25">
+        <v>0.67</v>
+      </c>
+      <c r="F25">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G25">
+        <v>0.36</v>
+      </c>
+      <c r="H25">
+        <v>1.19</v>
+      </c>
+      <c r="I25" t="s">
+        <v>74</v>
+      </c>
+      <c r="J25">
+        <v>18</v>
+      </c>
+      <c r="K25" t="s">
+        <v>100</v>
+      </c>
+      <c r="L25" t="s">
+        <v>110</v>
+      </c>
+      <c r="M25" t="s">
+        <v>90</v>
+      </c>
+      <c r="N25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>7</v>
+      </c>
+      <c r="B26">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>0.67</v>
+      </c>
+      <c r="F26">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G26">
+        <v>5.08</v>
+      </c>
+      <c r="H26">
+        <v>1.19</v>
+      </c>
+      <c r="I26" t="s">
+        <v>74</v>
+      </c>
+      <c r="J26">
+        <v>18</v>
+      </c>
+      <c r="K26" t="s">
+        <v>100</v>
+      </c>
+      <c r="L26" t="s">
+        <v>110</v>
+      </c>
+      <c r="M26" t="s">
+        <v>90</v>
+      </c>
+      <c r="N26" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>7</v>
+      </c>
+      <c r="B27">
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
         <v>108</v>
       </c>
-      <c r="D22">
-        <v>3</v>
-      </c>
-      <c r="E22">
+      <c r="D27">
+        <v>4</v>
+      </c>
+      <c r="E27">
         <v>0.34</v>
       </c>
-      <c r="F22">
+      <c r="F27">
         <v>2.31</v>
       </c>
-      <c r="G22">
+      <c r="G27">
         <v>6.73</v>
       </c>
-      <c r="H22">
+      <c r="H27">
         <v>6.78</v>
       </c>
-      <c r="I22" t="s">
-        <v>74</v>
-      </c>
-      <c r="J22">
+      <c r="I27" t="s">
+        <v>74</v>
+      </c>
+      <c r="J27">
         <v>14</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K27" t="s">
         <v>100</v>
       </c>
-      <c r="L22" s="2" t="str">
+      <c r="L27" s="2" t="str">
         <f>"202,202,202"</f>
         <v>202,202,202</v>
       </c>
-      <c r="M22" t="s">
+      <c r="M27" t="s">
         <v>109</v>
       </c>
-      <c r="O22" t="s">
+      <c r="O27" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>9</v>
-      </c>
-      <c r="B23">
-        <v>22</v>
-      </c>
-      <c r="C23" t="s">
-        <v>72</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <v>0.71</v>
-      </c>
-      <c r="F23">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="G23">
-        <v>0.15</v>
-      </c>
-      <c r="H23">
-        <v>0.15</v>
-      </c>
-      <c r="I23" t="s">
-        <v>74</v>
-      </c>
-      <c r="J23">
-        <v>40</v>
-      </c>
-      <c r="K23" t="s">
-        <v>100</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="M23" t="s">
-        <v>90</v>
-      </c>
-      <c r="N23" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>4</v>
-      </c>
-      <c r="B24">
-        <v>24</v>
-      </c>
-      <c r="C24" t="s">
-        <v>112</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="F24">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="G24">
-        <v>1.25</v>
-      </c>
-      <c r="H24">
-        <v>2.58</v>
-      </c>
-      <c r="I24" t="s">
-        <v>74</v>
-      </c>
-      <c r="J24">
-        <v>48</v>
-      </c>
-      <c r="K24" t="s">
-        <v>100</v>
-      </c>
-      <c r="L24" s="2" t="str">
-        <f>"255,255,255"</f>
-        <v>255,255,255</v>
-      </c>
-      <c r="M24" t="s">
-        <v>90</v>
-      </c>
-      <c r="N24" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>4</v>
-      </c>
-      <c r="B25">
-        <v>25</v>
-      </c>
-      <c r="C25" t="s">
-        <v>113</v>
-      </c>
-      <c r="D25">
-        <v>2</v>
-      </c>
-      <c r="E25">
-        <v>0.16</v>
-      </c>
-      <c r="F25">
-        <v>6.02</v>
-      </c>
-      <c r="G25">
-        <v>1.25</v>
-      </c>
-      <c r="H25">
-        <v>3.44</v>
-      </c>
-      <c r="I25" t="s">
-        <v>74</v>
-      </c>
-      <c r="J25">
-        <v>30</v>
-      </c>
-      <c r="K25" t="s">
-        <v>100</v>
-      </c>
-      <c r="L25" s="2" t="str">
-        <f>"255,255,255"</f>
-        <v>255,255,255</v>
-      </c>
-      <c r="M25" t="s">
-        <v>90</v>
-      </c>
-      <c r="N25" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>4</v>
-      </c>
-      <c r="B26">
-        <v>26</v>
-      </c>
-      <c r="C26" t="s">
-        <v>114</v>
-      </c>
-      <c r="D26">
-        <v>3</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="G26">
-        <v>1.25</v>
-      </c>
-      <c r="H26">
-        <v>4.05</v>
-      </c>
-      <c r="I26" t="s">
-        <v>74</v>
-      </c>
-      <c r="J26">
-        <v>30</v>
-      </c>
-      <c r="K26" t="s">
-        <v>100</v>
-      </c>
-      <c r="L26" s="2" t="str">
-        <f>"255,255,255"</f>
-        <v>255,255,255</v>
-      </c>
-      <c r="M26" t="s">
-        <v>90</v>
-      </c>
-      <c r="N26" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>11</v>
-      </c>
-      <c r="B27">
-        <v>27</v>
-      </c>
-      <c r="C27" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>0.71</v>
-      </c>
-      <c r="F27">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="G27">
-        <v>0.15</v>
-      </c>
-      <c r="H27">
-        <v>0.15</v>
-      </c>
-      <c r="I27" t="s">
-        <v>74</v>
-      </c>
-      <c r="J27">
-        <v>40</v>
-      </c>
-      <c r="K27" t="s">
-        <v>100</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="M27" t="s">
-        <v>90</v>
-      </c>
-      <c r="N27" t="s">
-        <v>119</v>
-      </c>
-      <c r="O27" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B28">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="C28" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E28">
-        <v>0.67</v>
+        <v>0.3</v>
       </c>
       <c r="F28">
-        <v>9.15</v>
+        <v>1.5</v>
       </c>
       <c r="G28">
-        <v>0.15</v>
+        <v>1.38</v>
       </c>
       <c r="H28">
-        <v>0.74</v>
+        <v>1.67</v>
       </c>
       <c r="I28" t="s">
         <v>74</v>
       </c>
       <c r="J28">
-        <v>28</v>
-      </c>
-      <c r="K28" t="s">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="M28" t="s">
         <v>90</v>
       </c>
       <c r="N28" t="s">
-        <v>136</v>
-      </c>
-      <c r="O28" t="s">
-        <v>101</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B29">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="C29" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="D29">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E29">
-        <v>0.34</v>
+        <v>0.3</v>
       </c>
       <c r="F29">
-        <v>2.31</v>
+        <v>1.5</v>
       </c>
       <c r="G29">
-        <v>6.73</v>
+        <v>5.37</v>
       </c>
       <c r="H29">
-        <v>6.78</v>
+        <v>1.67</v>
       </c>
       <c r="I29" t="s">
         <v>74</v>
       </c>
       <c r="J29">
-        <v>14</v>
-      </c>
-      <c r="K29" t="s">
-        <v>100</v>
-      </c>
-      <c r="L29" s="2" t="str">
-        <f>"202,202,202"</f>
-        <v>202,202,202</v>
+        <v>12</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="M29" t="s">
-        <v>109</v>
-      </c>
-      <c r="O29" t="s">
-        <v>101</v>
+        <v>90</v>
+      </c>
+      <c r="N29" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B30">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C30" t="s">
         <v>72</v>
@@ -3364,7 +3359,7 @@
         <v>0.71</v>
       </c>
       <c r="F30">
-        <v>8.4700000000000006</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="G30">
         <v>0.15</v>
@@ -3388,15 +3383,15 @@
         <v>90</v>
       </c>
       <c r="N30" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B31">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C31" t="s">
         <v>111</v>
@@ -3408,7 +3403,7 @@
         <v>0.67</v>
       </c>
       <c r="F31">
-        <v>9.15</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="G31">
         <v>0.15</v>
@@ -3432,7 +3427,7 @@
         <v>90</v>
       </c>
       <c r="N31" t="s">
-        <v>136</v>
+        <v>102</v>
       </c>
       <c r="O31" t="s">
         <v>101</v>
@@ -3440,10 +3435,10 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B32">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C32" t="s">
         <v>108</v>
@@ -3485,285 +3480,282 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B33">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C33" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="D33">
         <v>4</v>
       </c>
       <c r="E33">
-        <v>1.05</v>
+        <v>0.3</v>
       </c>
       <c r="F33">
+        <v>1.19</v>
+      </c>
+      <c r="G33">
+        <v>3.3</v>
+      </c>
+      <c r="H33">
+        <v>1.53</v>
+      </c>
+      <c r="I33" t="s">
+        <v>74</v>
+      </c>
+      <c r="J33">
+        <v>12</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="M33" t="s">
+        <v>90</v>
+      </c>
+      <c r="N33" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>9</v>
+      </c>
+      <c r="B34">
+        <v>22</v>
+      </c>
+      <c r="C34" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>0.71</v>
+      </c>
+      <c r="F34">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="G34">
+        <v>0.15</v>
+      </c>
+      <c r="H34">
+        <v>0.15</v>
+      </c>
+      <c r="I34" t="s">
+        <v>74</v>
+      </c>
+      <c r="J34">
+        <v>40</v>
+      </c>
+      <c r="K34" t="s">
+        <v>100</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="M34" t="s">
+        <v>90</v>
+      </c>
+      <c r="N34" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>10</v>
+      </c>
+      <c r="B35">
+        <v>30</v>
+      </c>
+      <c r="C35" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>0.71</v>
+      </c>
+      <c r="F35">
         <v>8.4700000000000006</v>
       </c>
-      <c r="G33">
-        <v>0.83</v>
-      </c>
-      <c r="H33">
-        <v>5.57</v>
-      </c>
-      <c r="I33" t="s">
-        <v>74</v>
-      </c>
-      <c r="J33">
+      <c r="G35">
+        <v>0.15</v>
+      </c>
+      <c r="H35">
+        <v>0.15</v>
+      </c>
+      <c r="I35" t="s">
+        <v>74</v>
+      </c>
+      <c r="J35">
+        <v>40</v>
+      </c>
+      <c r="K35" t="s">
+        <v>100</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="M35" t="s">
+        <v>90</v>
+      </c>
+      <c r="N35" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>10</v>
+      </c>
+      <c r="B36">
+        <v>31</v>
+      </c>
+      <c r="C36" t="s">
+        <v>111</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36">
+        <v>0.67</v>
+      </c>
+      <c r="F36">
+        <v>9.15</v>
+      </c>
+      <c r="G36">
+        <v>0.15</v>
+      </c>
+      <c r="H36">
+        <v>0.74</v>
+      </c>
+      <c r="I36" t="s">
+        <v>74</v>
+      </c>
+      <c r="J36">
+        <v>28</v>
+      </c>
+      <c r="K36" t="s">
+        <v>100</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="M36" t="s">
+        <v>90</v>
+      </c>
+      <c r="N36" t="s">
+        <v>136</v>
+      </c>
+      <c r="O36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>10</v>
+      </c>
+      <c r="B37">
+        <v>32</v>
+      </c>
+      <c r="C37" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37">
+        <v>3</v>
+      </c>
+      <c r="E37">
+        <v>0.34</v>
+      </c>
+      <c r="F37">
+        <v>2.31</v>
+      </c>
+      <c r="G37">
+        <v>6.73</v>
+      </c>
+      <c r="H37">
+        <v>6.78</v>
+      </c>
+      <c r="I37" t="s">
+        <v>74</v>
+      </c>
+      <c r="J37">
         <v>14</v>
       </c>
-      <c r="L33" s="2" t="str">
+      <c r="K37" t="s">
+        <v>100</v>
+      </c>
+      <c r="L37" s="2" t="str">
         <f>"202,202,202"</f>
         <v>202,202,202</v>
       </c>
-      <c r="M33" t="s">
-        <v>90</v>
-      </c>
-      <c r="N33" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>11</v>
-      </c>
-      <c r="B34">
-        <v>34</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="M37" t="s">
+        <v>109</v>
+      </c>
+      <c r="O37" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>10</v>
+      </c>
+      <c r="B38">
+        <v>33</v>
+      </c>
+      <c r="C38" t="s">
         <v>120</v>
       </c>
-      <c r="D34">
+      <c r="D38">
         <v>4</v>
       </c>
-      <c r="E34">
+      <c r="E38">
         <v>1.05</v>
       </c>
-      <c r="F34">
+      <c r="F38">
         <v>8.4700000000000006</v>
       </c>
-      <c r="G34">
+      <c r="G38">
         <v>0.83</v>
       </c>
-      <c r="H34">
+      <c r="H38">
         <v>5.57</v>
       </c>
-      <c r="I34" t="s">
-        <v>74</v>
-      </c>
-      <c r="J34">
+      <c r="I38" t="s">
+        <v>74</v>
+      </c>
+      <c r="J38">
         <v>14</v>
       </c>
-      <c r="L34" s="2" t="str">
+      <c r="L38" s="2" t="str">
         <f>"202,202,202"</f>
         <v>202,202,202</v>
       </c>
-      <c r="M34" t="s">
-        <v>90</v>
-      </c>
-      <c r="N34" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>5</v>
-      </c>
-      <c r="B35">
-        <v>35</v>
-      </c>
-      <c r="C35" t="s">
-        <v>112</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35">
-        <v>1</v>
-      </c>
-      <c r="F35">
-        <v>7.76</v>
-      </c>
-      <c r="G35">
-        <v>1.25</v>
-      </c>
-      <c r="H35">
-        <v>2.58</v>
-      </c>
-      <c r="I35" t="s">
-        <v>74</v>
-      </c>
-      <c r="J35">
-        <v>48</v>
-      </c>
-      <c r="K35" t="s">
-        <v>100</v>
-      </c>
-      <c r="L35" s="2" t="str">
-        <f>"255,255,255"</f>
-        <v>255,255,255</v>
-      </c>
-      <c r="M35" t="s">
-        <v>90</v>
-      </c>
-      <c r="N35" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>5</v>
-      </c>
-      <c r="B36">
-        <v>36</v>
-      </c>
-      <c r="C36" t="s">
-        <v>113</v>
-      </c>
-      <c r="D36">
-        <v>2</v>
-      </c>
-      <c r="E36">
-        <v>0.16</v>
-      </c>
-      <c r="F36">
-        <v>6.02</v>
-      </c>
-      <c r="G36">
-        <v>1.25</v>
-      </c>
-      <c r="H36">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="I36" t="s">
-        <v>74</v>
-      </c>
-      <c r="J36">
-        <v>30</v>
-      </c>
-      <c r="K36" t="s">
-        <v>100</v>
-      </c>
-      <c r="L36" s="2" t="str">
-        <f>"255,255,255"</f>
-        <v>255,255,255</v>
-      </c>
-      <c r="M36" t="s">
-        <v>90</v>
-      </c>
-      <c r="N36" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>5</v>
-      </c>
-      <c r="B37">
-        <v>37</v>
-      </c>
-      <c r="C37" t="s">
-        <v>114</v>
-      </c>
-      <c r="D37">
-        <v>3</v>
-      </c>
-      <c r="E37">
-        <v>1</v>
-      </c>
-      <c r="F37">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="G37">
-        <v>1.25</v>
-      </c>
-      <c r="H37">
-        <v>4.71</v>
-      </c>
-      <c r="I37" t="s">
-        <v>74</v>
-      </c>
-      <c r="J37">
-        <v>30</v>
-      </c>
-      <c r="K37" t="s">
-        <v>100</v>
-      </c>
-      <c r="L37" s="2" t="str">
-        <f>"255,255,255"</f>
-        <v>255,255,255</v>
-      </c>
-      <c r="M37" t="s">
-        <v>90</v>
-      </c>
-      <c r="O37" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>12</v>
-      </c>
-      <c r="B38">
-        <v>38</v>
-      </c>
-      <c r="C38" t="s">
-        <v>72</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38">
-        <v>0.71</v>
-      </c>
-      <c r="F38">
-        <v>9.4600000000000009</v>
-      </c>
-      <c r="G38">
-        <v>0.15</v>
-      </c>
-      <c r="H38">
-        <v>0.15</v>
-      </c>
-      <c r="I38" t="s">
-        <v>74</v>
-      </c>
-      <c r="J38">
-        <v>40</v>
-      </c>
-      <c r="K38" t="s">
-        <v>100</v>
-      </c>
-      <c r="L38" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="M38" t="s">
         <v>90</v>
       </c>
       <c r="N38" t="s">
-        <v>124</v>
-      </c>
-      <c r="O38" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B39">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C39" t="s">
-        <v>111</v>
+        <v>72</v>
       </c>
       <c r="D39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E39">
-        <v>0.67</v>
+        <v>0.71</v>
       </c>
       <c r="F39">
         <v>9.1999999999999993</v>
@@ -3772,13 +3764,13 @@
         <v>0.15</v>
       </c>
       <c r="H39">
-        <v>0.74</v>
+        <v>0.15</v>
       </c>
       <c r="I39" t="s">
         <v>74</v>
       </c>
       <c r="J39">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="K39" t="s">
         <v>100</v>
@@ -3789,59 +3781,413 @@
       <c r="M39" t="s">
         <v>90</v>
       </c>
+      <c r="N39" t="s">
+        <v>119</v>
+      </c>
       <c r="O39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B40">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C40" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D40">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E40">
-        <v>0.34</v>
+        <v>0.67</v>
       </c>
       <c r="F40">
-        <v>2.31</v>
+        <v>9.15</v>
       </c>
       <c r="G40">
-        <v>6.73</v>
+        <v>0.15</v>
       </c>
       <c r="H40">
-        <v>6.78</v>
+        <v>0.74</v>
       </c>
       <c r="I40" t="s">
         <v>74</v>
       </c>
       <c r="J40">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="K40" t="s">
         <v>100</v>
       </c>
-      <c r="L40" s="2" t="str">
+      <c r="L40" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="M40" t="s">
+        <v>90</v>
+      </c>
+      <c r="N40" t="s">
+        <v>136</v>
+      </c>
+      <c r="O40" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>11</v>
+      </c>
+      <c r="B41">
+        <v>29</v>
+      </c>
+      <c r="C41" t="s">
+        <v>108</v>
+      </c>
+      <c r="D41">
+        <v>3</v>
+      </c>
+      <c r="E41">
+        <v>0.34</v>
+      </c>
+      <c r="F41">
+        <v>2.31</v>
+      </c>
+      <c r="G41">
+        <v>6.73</v>
+      </c>
+      <c r="H41">
+        <v>6.78</v>
+      </c>
+      <c r="I41" t="s">
+        <v>74</v>
+      </c>
+      <c r="J41">
+        <v>14</v>
+      </c>
+      <c r="K41" t="s">
+        <v>100</v>
+      </c>
+      <c r="L41" s="2" t="str">
         <f>"202,202,202"</f>
         <v>202,202,202</v>
       </c>
-      <c r="M40" t="s">
+      <c r="M41" t="s">
         <v>109</v>
       </c>
-      <c r="O40" t="s">
+      <c r="O41" t="s">
         <v>101</v>
       </c>
     </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>11</v>
+      </c>
+      <c r="B42">
+        <v>34</v>
+      </c>
+      <c r="C42" t="s">
+        <v>120</v>
+      </c>
+      <c r="D42">
+        <v>4</v>
+      </c>
+      <c r="E42">
+        <v>1.05</v>
+      </c>
+      <c r="F42">
+        <v>8.4700000000000006</v>
+      </c>
+      <c r="G42">
+        <v>0.83</v>
+      </c>
+      <c r="H42">
+        <v>5.57</v>
+      </c>
+      <c r="I42" t="s">
+        <v>74</v>
+      </c>
+      <c r="J42">
+        <v>14</v>
+      </c>
+      <c r="L42" s="2" t="str">
+        <f>"202,202,202"</f>
+        <v>202,202,202</v>
+      </c>
+      <c r="M42" t="s">
+        <v>90</v>
+      </c>
+      <c r="N42" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>12</v>
+      </c>
+      <c r="B43">
+        <v>38</v>
+      </c>
+      <c r="C43" t="s">
+        <v>72</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>0.71</v>
+      </c>
+      <c r="F43">
+        <v>9.4600000000000009</v>
+      </c>
+      <c r="G43">
+        <v>0.15</v>
+      </c>
+      <c r="H43">
+        <v>0.15</v>
+      </c>
+      <c r="I43" t="s">
+        <v>74</v>
+      </c>
+      <c r="J43">
+        <v>40</v>
+      </c>
+      <c r="K43" t="s">
+        <v>100</v>
+      </c>
+      <c r="L43" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="M43" t="s">
+        <v>90</v>
+      </c>
+      <c r="N43" t="s">
+        <v>124</v>
+      </c>
+      <c r="O43" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>12</v>
+      </c>
+      <c r="B44">
+        <v>39</v>
+      </c>
+      <c r="C44" t="s">
+        <v>111</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="E44">
+        <v>0.67</v>
+      </c>
+      <c r="F44">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="G44">
+        <v>0.15</v>
+      </c>
+      <c r="H44">
+        <v>0.74</v>
+      </c>
+      <c r="I44" t="s">
+        <v>74</v>
+      </c>
+      <c r="J44">
+        <v>28</v>
+      </c>
+      <c r="K44" t="s">
+        <v>100</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="M44" t="s">
+        <v>90</v>
+      </c>
+      <c r="O44" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>12</v>
+      </c>
+      <c r="B45">
+        <v>40</v>
+      </c>
+      <c r="C45" t="s">
+        <v>108</v>
+      </c>
+      <c r="D45">
+        <v>3</v>
+      </c>
+      <c r="E45">
+        <v>0.34</v>
+      </c>
+      <c r="F45">
+        <v>2.31</v>
+      </c>
+      <c r="G45">
+        <v>6.73</v>
+      </c>
+      <c r="H45">
+        <v>6.78</v>
+      </c>
+      <c r="I45" t="s">
+        <v>74</v>
+      </c>
+      <c r="J45">
+        <v>14</v>
+      </c>
+      <c r="K45" t="s">
+        <v>100</v>
+      </c>
+      <c r="L45" s="2" t="str">
+        <f>"202,202,202"</f>
+        <v>202,202,202</v>
+      </c>
+      <c r="M45" t="s">
+        <v>109</v>
+      </c>
+      <c r="O45" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>9</v>
+      </c>
+      <c r="B46">
+        <v>46</v>
+      </c>
+      <c r="C46" t="s">
+        <v>139</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46">
+        <v>0.3</v>
+      </c>
+      <c r="F46">
+        <v>1.19</v>
+      </c>
+      <c r="G46">
+        <v>3.27</v>
+      </c>
+      <c r="H46">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="I46" t="s">
+        <v>74</v>
+      </c>
+      <c r="J46">
+        <v>12</v>
+      </c>
+      <c r="L46" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="M46" t="s">
+        <v>90</v>
+      </c>
+      <c r="N46" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>10</v>
+      </c>
+      <c r="B47">
+        <v>47</v>
+      </c>
+      <c r="C47" t="s">
+        <v>139</v>
+      </c>
+      <c r="D47">
+        <v>5</v>
+      </c>
+      <c r="E47">
+        <v>0.3</v>
+      </c>
+      <c r="F47">
+        <v>1.5</v>
+      </c>
+      <c r="G47">
+        <v>2.8</v>
+      </c>
+      <c r="H47">
+        <v>1.41</v>
+      </c>
+      <c r="I47" t="s">
+        <v>74</v>
+      </c>
+      <c r="J47">
+        <v>12</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="M47" t="s">
+        <v>90</v>
+      </c>
+      <c r="N47" t="str">
+        <f>"-- state average"</f>
+        <v>-- state average</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>11</v>
+      </c>
+      <c r="B48">
+        <v>48</v>
+      </c>
+      <c r="C48" t="s">
+        <v>139</v>
+      </c>
+      <c r="D48">
+        <v>5</v>
+      </c>
+      <c r="E48">
+        <v>0.3</v>
+      </c>
+      <c r="F48">
+        <v>1.5</v>
+      </c>
+      <c r="G48">
+        <v>2.8</v>
+      </c>
+      <c r="H48">
+        <v>1.41</v>
+      </c>
+      <c r="I48" t="s">
+        <v>74</v>
+      </c>
+      <c r="J48">
+        <v>12</v>
+      </c>
+      <c r="L48" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="M48" t="s">
+        <v>90</v>
+      </c>
+      <c r="N48" t="str">
+        <f>"-- state average"</f>
+        <v>-- state average</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:O6">
-    <sortCondition ref="A2:A6"/>
-    <sortCondition ref="D2:D6"/>
+  <autoFilter ref="A1:O48" xr:uid="{5D5DEDAD-75E1-4247-A1F5-DD579159CD80}"/>
+  <sortState ref="A2:O45">
+    <sortCondition ref="A2:A45"/>
+    <sortCondition ref="D2:D45"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed two small text issues removing "SY" and adding numbering on second slide.
</commit_message>
<xml_diff>
--- a/graph_configs.xlsx
+++ b/graph_configs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WNF\Documents\GIT PROJECTS\CWIS-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D7991C-81B1-45EB-AB90-26EA39BE276A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E584F635-F234-4821-8C42-09559AEE13F8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="7710" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="143">
   <si>
     <t>slide.type.id</t>
   </si>
@@ -304,9 +304,6 @@
     <t>Repeated Measures Report</t>
   </si>
   <si>
-    <t>Baseline through 2017-18 SY</t>
-  </si>
-  <si>
     <t>left</t>
   </si>
   <si>
@@ -440,6 +437,30 @@
   </si>
   <si>
     <t>Baseline through 2017-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baseline through 2017-18: </t>
+  </si>
+  <si>
+    <t>Documented above are the percent of school respondents who answered that they use MMD practices. "For some essential functions, 'use' is determined by reported frequency (e.g. 'most of the time' or 'always'); for other functions, 'use' is determined through agreement (e.g. 'agree' or 'strongly agree'). Please see Green Reports for a list of complete prompts.</t>
+  </si>
+  <si>
+    <t>Documented above are the percent of school respondents who answered that they use MMD practices. For some essential functions, 'use' is determined by reported frequency (e.g. 'most of the time' or 'always'); for other functions, 'use' is determined through agreement (e.g. 'agree' or 'strongly agree'). Please see Green Reports for a list of complete prompts.</t>
+  </si>
+  <si>
+    <t>average.legend.1</t>
+  </si>
+  <si>
+    <t>average.legend.2</t>
+  </si>
+  <si>
+    <t>l state average</t>
+  </si>
+  <si>
+    <t>0,0,0</t>
+  </si>
+  <si>
+    <t>l district average</t>
   </si>
   <si>
     <t>1. This is a district report that will show aggregated data by school level as well as disaggregated data by building.
@@ -447,31 +468,7 @@
 3. Implementation rates are presented as the rate of responses that marked either "most of the time" or "always" or "agree" or "strongly agree".
 4. Data are presented for five major activities: 1) Effective Teaching and Learning Practices, 2) Common Formative Assessment, 3) Data-based Decision-making, 4) Leadership, and, 5) Professional Development.
 5. State averages are presented for district aggregate charts, while district averages are presented on visuals for individual schools.
-Charts detailing implementation performance later in this report are presented "by response" so that the relative change in participation is also perceptible.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Baseline through 2017-18: </t>
-  </si>
-  <si>
-    <t>Documented above are the percent of school respondents who answered that they use MMD practices. "For some essential functions, 'use' is determined by reported frequency (e.g. 'most of the time' or 'always'); for other functions, 'use' is determined through agreement (e.g. 'agree' or 'strongly agree'). Please see Green Reports for a list of complete prompts.</t>
-  </si>
-  <si>
-    <t>Documented above are the percent of school respondents who answered that they use MMD practices. For some essential functions, 'use' is determined by reported frequency (e.g. 'most of the time' or 'always'); for other functions, 'use' is determined through agreement (e.g. 'agree' or 'strongly agree'). Please see Green Reports for a list of complete prompts.</t>
-  </si>
-  <si>
-    <t>average.legend.1</t>
-  </si>
-  <si>
-    <t>average.legend.2</t>
-  </si>
-  <si>
-    <t>l state average</t>
-  </si>
-  <si>
-    <t>0,0,0</t>
-  </si>
-  <si>
-    <t>l district average</t>
+6. Charts detailing implementation performance later in this report are presented "by response" so that the relative change in participation is also perceptible.</t>
   </si>
 </sst>
 </file>
@@ -966,7 +963,9 @@
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1620,16 +1619,16 @@
         <v>37</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -1637,7 +1636,7 @@
         <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
@@ -1772,7 +1771,7 @@
         <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C5" t="s">
         <v>39</v>
@@ -1863,7 +1862,7 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C7" t="s">
         <v>39</v>
@@ -1907,7 +1906,7 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C8" t="s">
         <v>57</v>
@@ -1951,7 +1950,7 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C9" t="s">
         <v>57</v>
@@ -2051,8 +2050,8 @@
   <dimension ref="A1:O48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2079,16 +2078,16 @@
         <v>62</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>69</v>
@@ -2097,13 +2096,13 @@
         <v>70</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>85</v>
@@ -2144,13 +2143,13 @@
         <v>48</v>
       </c>
       <c r="K2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N2" t="s">
         <v>88</v>
@@ -2192,13 +2191,13 @@
         <v>230,230,230</v>
       </c>
       <c r="M3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="O3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -2233,19 +2232,19 @@
         <v>28</v>
       </c>
       <c r="K4" t="s">
+        <v>99</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="M4" t="s">
+        <v>89</v>
+      </c>
+      <c r="N4" t="s">
+        <v>101</v>
+      </c>
+      <c r="O4" t="s">
         <v>100</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="M4" t="s">
-        <v>90</v>
-      </c>
-      <c r="N4" t="s">
-        <v>102</v>
-      </c>
-      <c r="O4" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -2280,13 +2279,13 @@
         <v>30</v>
       </c>
       <c r="L5" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="M5" t="s">
+        <v>89</v>
+      </c>
+      <c r="N5" t="s">
         <v>133</v>
-      </c>
-      <c r="M5" t="s">
-        <v>90</v>
-      </c>
-      <c r="N5" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -2321,16 +2320,16 @@
         <v>30</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -2338,7 +2337,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -2362,10 +2361,10 @@
         <v>14</v>
       </c>
       <c r="M7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -2376,7 +2375,7 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -2400,17 +2399,17 @@
         <v>14</v>
       </c>
       <c r="K8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L8" s="2" t="str">
         <f>"202,202,202"</f>
         <v>202,202,202</v>
       </c>
       <c r="M8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -2421,7 +2420,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -2445,17 +2444,17 @@
         <v>48</v>
       </c>
       <c r="K9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L9" s="2" t="str">
-        <f>"255,255,255"</f>
+        <f t="shared" ref="L9:L17" si="0">"255,255,255"</f>
         <v>255,255,255</v>
       </c>
       <c r="M9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -2466,7 +2465,7 @@
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -2490,17 +2489,17 @@
         <v>30</v>
       </c>
       <c r="K10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L10" s="2" t="str">
-        <f>"255,255,255"</f>
+        <f t="shared" si="0"/>
         <v>255,255,255</v>
       </c>
       <c r="M10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -2511,7 +2510,7 @@
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D11">
         <v>3</v>
@@ -2535,17 +2534,17 @@
         <v>30</v>
       </c>
       <c r="K11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L11" s="2" t="str">
-        <f>"255,255,255"</f>
+        <f t="shared" si="0"/>
         <v>255,255,255</v>
       </c>
       <c r="M11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -2556,7 +2555,7 @@
         <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -2580,17 +2579,17 @@
         <v>48</v>
       </c>
       <c r="K12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L12" s="2" t="str">
-        <f>"255,255,255"</f>
+        <f t="shared" si="0"/>
         <v>255,255,255</v>
       </c>
       <c r="M12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2601,7 +2600,7 @@
         <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -2625,17 +2624,17 @@
         <v>30</v>
       </c>
       <c r="K13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L13" s="2" t="str">
-        <f>"255,255,255"</f>
+        <f t="shared" si="0"/>
         <v>255,255,255</v>
       </c>
       <c r="M13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -2646,7 +2645,7 @@
         <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D14">
         <v>3</v>
@@ -2670,17 +2669,17 @@
         <v>30</v>
       </c>
       <c r="K14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L14" s="2" t="str">
-        <f>"255,255,255"</f>
+        <f t="shared" si="0"/>
         <v>255,255,255</v>
       </c>
       <c r="M14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -2691,7 +2690,7 @@
         <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -2715,17 +2714,17 @@
         <v>48</v>
       </c>
       <c r="K15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L15" s="2" t="str">
-        <f>"255,255,255"</f>
+        <f t="shared" si="0"/>
         <v>255,255,255</v>
       </c>
       <c r="M15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -2736,7 +2735,7 @@
         <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -2760,17 +2759,17 @@
         <v>30</v>
       </c>
       <c r="K16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L16" s="2" t="str">
-        <f>"255,255,255"</f>
+        <f t="shared" si="0"/>
         <v>255,255,255</v>
       </c>
       <c r="M16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -2781,7 +2780,7 @@
         <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D17">
         <v>3</v>
@@ -2805,17 +2804,17 @@
         <v>30</v>
       </c>
       <c r="K17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L17" s="2" t="str">
-        <f>"255,255,255"</f>
+        <f t="shared" si="0"/>
         <v>255,255,255</v>
       </c>
       <c r="M17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -2850,19 +2849,19 @@
         <v>30</v>
       </c>
       <c r="K18" t="s">
+        <v>99</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="M18" t="s">
+        <v>89</v>
+      </c>
+      <c r="N18" t="s">
+        <v>104</v>
+      </c>
+      <c r="O18" t="s">
         <v>100</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="M18" t="s">
-        <v>90</v>
-      </c>
-      <c r="N18" t="s">
-        <v>105</v>
-      </c>
-      <c r="O18" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -2873,7 +2872,7 @@
         <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -2897,16 +2896,16 @@
         <v>18</v>
       </c>
       <c r="K19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -2917,7 +2916,7 @@
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D20">
         <v>3</v>
@@ -2941,16 +2940,16 @@
         <v>18</v>
       </c>
       <c r="K20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -2961,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D21">
         <v>4</v>
@@ -2985,17 +2984,17 @@
         <v>14</v>
       </c>
       <c r="K21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L21" s="2" t="str">
         <f>"202,202,202"</f>
         <v>202,202,202</v>
       </c>
       <c r="M21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -3006,7 +3005,7 @@
         <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D22">
         <v>5</v>
@@ -3030,13 +3029,13 @@
         <v>12</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="M22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N22" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -3047,7 +3046,7 @@
         <v>42</v>
       </c>
       <c r="C23" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D23">
         <v>6</v>
@@ -3071,13 +3070,13 @@
         <v>12</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="M23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N23" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -3112,19 +3111,19 @@
         <v>30</v>
       </c>
       <c r="K24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -3135,7 +3134,7 @@
         <v>12</v>
       </c>
       <c r="C25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D25">
         <v>2</v>
@@ -3159,16 +3158,16 @@
         <v>18</v>
       </c>
       <c r="K25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -3179,7 +3178,7 @@
         <v>13</v>
       </c>
       <c r="C26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D26">
         <v>3</v>
@@ -3203,16 +3202,16 @@
         <v>18</v>
       </c>
       <c r="K26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -3223,7 +3222,7 @@
         <v>14</v>
       </c>
       <c r="C27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D27">
         <v>4</v>
@@ -3247,17 +3246,17 @@
         <v>14</v>
       </c>
       <c r="K27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L27" s="2" t="str">
         <f>"202,202,202"</f>
         <v>202,202,202</v>
       </c>
       <c r="M27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -3268,7 +3267,7 @@
         <v>43</v>
       </c>
       <c r="C28" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D28">
         <v>5</v>
@@ -3292,13 +3291,13 @@
         <v>12</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="M28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N28" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -3309,7 +3308,7 @@
         <v>44</v>
       </c>
       <c r="C29" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D29">
         <v>6</v>
@@ -3333,13 +3332,13 @@
         <v>12</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="M29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N29" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -3374,16 +3373,16 @@
         <v>40</v>
       </c>
       <c r="K30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -3394,7 +3393,7 @@
         <v>19</v>
       </c>
       <c r="C31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D31">
         <v>2</v>
@@ -3418,19 +3417,19 @@
         <v>28</v>
       </c>
       <c r="K31" t="s">
+        <v>99</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="M31" t="s">
+        <v>89</v>
+      </c>
+      <c r="N31" t="s">
+        <v>101</v>
+      </c>
+      <c r="O31" t="s">
         <v>100</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="M31" t="s">
-        <v>90</v>
-      </c>
-      <c r="N31" t="s">
-        <v>102</v>
-      </c>
-      <c r="O31" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -3441,7 +3440,7 @@
         <v>20</v>
       </c>
       <c r="C32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D32">
         <v>3</v>
@@ -3465,17 +3464,17 @@
         <v>14</v>
       </c>
       <c r="K32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L32" s="2" t="str">
         <f>"202,202,202"</f>
         <v>202,202,202</v>
       </c>
       <c r="M32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -3486,7 +3485,7 @@
         <v>45</v>
       </c>
       <c r="C33" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D33">
         <v>4</v>
@@ -3510,13 +3509,13 @@
         <v>12</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="M33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N33" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
@@ -3551,16 +3550,16 @@
         <v>40</v>
       </c>
       <c r="K34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N34" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
@@ -3595,16 +3594,16 @@
         <v>40</v>
       </c>
       <c r="K35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N35" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
@@ -3615,7 +3614,7 @@
         <v>31</v>
       </c>
       <c r="C36" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D36">
         <v>2</v>
@@ -3639,19 +3638,19 @@
         <v>28</v>
       </c>
       <c r="K36" t="s">
+        <v>99</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="M36" t="s">
+        <v>89</v>
+      </c>
+      <c r="N36" t="s">
+        <v>134</v>
+      </c>
+      <c r="O36" t="s">
         <v>100</v>
-      </c>
-      <c r="L36" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="M36" t="s">
-        <v>90</v>
-      </c>
-      <c r="N36" t="s">
-        <v>136</v>
-      </c>
-      <c r="O36" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
@@ -3662,7 +3661,7 @@
         <v>32</v>
       </c>
       <c r="C37" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D37">
         <v>3</v>
@@ -3686,17 +3685,17 @@
         <v>14</v>
       </c>
       <c r="K37" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L37" s="2" t="str">
         <f>"202,202,202"</f>
         <v>202,202,202</v>
       </c>
       <c r="M37" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
@@ -3707,7 +3706,7 @@
         <v>33</v>
       </c>
       <c r="C38" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D38">
         <v>4</v>
@@ -3735,10 +3734,10 @@
         <v>202,202,202</v>
       </c>
       <c r="M38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N38" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
@@ -3773,19 +3772,19 @@
         <v>40</v>
       </c>
       <c r="K39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M39" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N39" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O39" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
@@ -3796,7 +3795,7 @@
         <v>28</v>
       </c>
       <c r="C40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D40">
         <v>2</v>
@@ -3820,19 +3819,19 @@
         <v>28</v>
       </c>
       <c r="K40" t="s">
+        <v>99</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="M40" t="s">
+        <v>89</v>
+      </c>
+      <c r="N40" t="s">
+        <v>134</v>
+      </c>
+      <c r="O40" t="s">
         <v>100</v>
-      </c>
-      <c r="L40" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="M40" t="s">
-        <v>90</v>
-      </c>
-      <c r="N40" t="s">
-        <v>136</v>
-      </c>
-      <c r="O40" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
@@ -3843,7 +3842,7 @@
         <v>29</v>
       </c>
       <c r="C41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D41">
         <v>3</v>
@@ -3867,17 +3866,17 @@
         <v>14</v>
       </c>
       <c r="K41" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L41" s="2" t="str">
         <f>"202,202,202"</f>
         <v>202,202,202</v>
       </c>
       <c r="M41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
@@ -3888,7 +3887,7 @@
         <v>34</v>
       </c>
       <c r="C42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D42">
         <v>4</v>
@@ -3916,10 +3915,10 @@
         <v>202,202,202</v>
       </c>
       <c r="M42" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N42" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
@@ -3954,19 +3953,19 @@
         <v>40</v>
       </c>
       <c r="K43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M43" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N43" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="O43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
@@ -3977,7 +3976,7 @@
         <v>39</v>
       </c>
       <c r="C44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D44">
         <v>2</v>
@@ -4001,16 +4000,16 @@
         <v>28</v>
       </c>
       <c r="K44" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M44" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O44" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
@@ -4021,7 +4020,7 @@
         <v>40</v>
       </c>
       <c r="C45" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D45">
         <v>3</v>
@@ -4045,17 +4044,17 @@
         <v>14</v>
       </c>
       <c r="K45" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L45" s="2" t="str">
         <f>"202,202,202"</f>
         <v>202,202,202</v>
       </c>
       <c r="M45" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
@@ -4066,7 +4065,7 @@
         <v>46</v>
       </c>
       <c r="C46" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D46">
         <v>2</v>
@@ -4090,13 +4089,13 @@
         <v>12</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="M46" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N46" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
@@ -4107,7 +4106,7 @@
         <v>47</v>
       </c>
       <c r="C47" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D47">
         <v>5</v>
@@ -4131,10 +4130,10 @@
         <v>12</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="M47" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N47" t="str">
         <f>"-- state average"</f>
@@ -4149,7 +4148,7 @@
         <v>48</v>
       </c>
       <c r="C48" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D48">
         <v>5</v>
@@ -4173,10 +4172,10 @@
         <v>12</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="M48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N48" t="str">
         <f>"-- state average"</f>

</xml_diff>

<commit_message>
Began updates to pull in data for Green Reports direct from Qualtrics
</commit_message>
<xml_diff>
--- a/graph_configs.xlsx
+++ b/graph_configs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WNF\Documents\GIT PROJECTS\CWIS-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E584F635-F234-4821-8C42-09559AEE13F8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8EBA25-8616-4868-B52A-A9A45F58BFCE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="7710" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
   </bookViews>
@@ -2050,7 +2050,7 @@
   <dimension ref="A1:O48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>

</xml_diff>